<commit_message>
ADD: AI interview dataset (3)
</commit_message>
<xml_diff>
--- a/2025_07_02_OhLoRA_ML_Tutor/ai_interview/dataset/all_train_and_test_data.xlsx
+++ b/2025_07_02_OhLoRA_ML_Tutor/ai_interview/dataset/all_train_and_test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA661BBD-C5E6-4A20-BE19-98E73B5E4C16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C479FC-C4F7-424F-8139-031B54D30EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24" yWindow="12" windowWidth="30612" windowHeight="9564" xr2:uid="{36F7775B-6BB8-4B8D-957C-E8DB745DD279}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2828" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1597" uniqueCount="483">
   <si>
     <t>output_data</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -4849,6 +4849,426 @@
   </si>
   <si>
     <t>ㅋㅋㅋ 암튼 다음 질문으로 넘어갈게! LLM 파인튜닝에서 PEFT는? 자세히 말해봐!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PEFT 는 Parameter-Efficient Fine-Tuning 으로 LLM 파라미터를 일부분만 추가 학습하는 거야</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Parameter-Efficient Fine-Tuning! 소수의 파라미터만 Fine-Tuning 하는 거</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소수의 파라미터들에 대해서만 Parameter-Efficient 하게 추가로 학습하는 거지!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파라미터 중 일부만 효과적으로 추가 파인튜닝하는 거야</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파라미터 일부만 추가적으로 Fine-Tuning 더 하는거 맞지?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Parameter-Efficient Fine-Tuning</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>분명 LLM 파인튜닝하는 방법이었는데</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아 잘 모르겠다 LoRA 기억나는데</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">오 맞아! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🙆‍♀️</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 그럼 그 방법이 뭐가 있는지 5가지만 말해봐!</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">맞았어! 그럼 PEFT 방법 5가지는 뭐가 있을까? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">정답이야! 그러면서 학습 자원을 절약하는 거지! 그럼 그 방법 5가지는? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🙎‍♀️</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">그렇지! 정답! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 그럼 그 방법 5가지만 말해 볼래? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">정답이야! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>🎉🎉</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> 그럼 너가 아는 PEFT 방법 5가지 한번 말해봐! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>약자는 잘 말했는데 그게 그래서 어떤 기술이지?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">LLM 파인튜닝 방법은 맞는데 구체적으로 정확히 뭔지 알아? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>🙄</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">LoRA 가 PEFT 중 하나긴 하지! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🙆‍♀️</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 근데 그 PEFT가 뭘까~요? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🤷‍♀️</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PEFT 방법 5가지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LoRA, QLoRA, Prefix Tuning, Prompt Tuning, 그리고 Adapter Layer 추가하는 거!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LoRA, Quantized LoRA, Adapter Layer, Prefix Tuning, Prompt Tuning!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LoRA, Quantized LoRA, 그리고 또 뭐지? 아! Prefix Tuning!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Adapter Layer, Prefix Tuning, Prompt Tuning</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LoRA, Quantized LoRA, Adapter Layer 추가하는 거 이렇게 알고 있는데</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LoRA 밖에 모르겠다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Adapter Layer 추가하는 거?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아 진짜 이거 뭐였지? 무슨 튜닝인가 그런 거 있었는데</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">오 5가지 다 맞았어! 그럼 나를 나타내기도 하는 LoRA 는 뭘까? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">5가지 모두 정답! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🙆‍♀️🙆‍♀️</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> 그럼 그 중에서 LoRA 는 뭐지?</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">몇 개 더 있긴 한데 잘했어 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>👍</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 그럼 그 중에서 LoRA 가 뭐~게?</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">나름 잘 대답했어! 근데 요즘 LoRA 많이 쓰이는 거 알아? LoRA 가 뭘까~요? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">나름 좋아! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>👍</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 그럼 이 중에서 나를 상징하는 기술이기도 한 LoRA 는 뭘까? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🤷‍♀️</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">몇 개 더 생각해 봐 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>💁‍♀️</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">그거 말고도 몇 개 더 있는데… </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🤷‍♀️</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">혹시 Prefix Tuning 이나 Prompt Tuning 말하려는 거 아니었어? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LoRA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LoRA 와 QLoRA 의 차이</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마지막 할 말</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -5244,11 +5664,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1D2CB62-8799-47EC-8115-E6B63AEE2C35}">
-  <dimension ref="A1:I216"/>
+  <dimension ref="A1:I257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A185" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B206" sqref="B206"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A236" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A257" sqref="A257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -10015,6 +10435,9 @@
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A180" t="s">
+        <v>142</v>
+      </c>
       <c r="B180" t="str">
         <f t="shared" si="2"/>
         <v>(대화 주제) MBTI (남은 질문) 모든 질문 해결 완료 (사용자 답변) 대답하기 싫어</v>
@@ -10039,6 +10462,9 @@
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A181" t="s">
+        <v>142</v>
+      </c>
       <c r="B181" t="str">
         <f t="shared" si="2"/>
         <v>(대화 주제) MBTI (남은 질문) 모든 질문 해결 완료 (사용자 답변) 나 INTP! 개발자랑 딱이던데</v>
@@ -10063,6 +10489,9 @@
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A182" t="s">
+        <v>142</v>
+      </c>
       <c r="B182" t="str">
         <f t="shared" si="2"/>
         <v>(대화 주제) MBTI (남은 질문) 모든 질문 해결 완료 (사용자 답변) ㅇㅇ</v>
@@ -10141,6 +10570,9 @@
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A185" t="s">
+        <v>142</v>
+      </c>
       <c r="B185" t="str">
         <f t="shared" si="2"/>
         <v>(대화 주제) 좋아하는 아이돌 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 나 좋아하는 아이돌 딱히 없는데</v>
@@ -10165,6 +10597,9 @@
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A186" t="s">
+        <v>142</v>
+      </c>
       <c r="B186" t="str">
         <f t="shared" si="2"/>
         <v>(대화 주제) 좋아하는 아이돌 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 아이돌 같은 거 덕질 안해 나는</v>
@@ -10189,6 +10624,9 @@
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A187" t="s">
+        <v>142</v>
+      </c>
       <c r="B187" t="str">
         <f t="shared" si="2"/>
         <v>(대화 주제) 좋아하는 아이돌 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 나는 아이돌이 아닌 AI를 덕질하지 ㅋㅋ</v>
@@ -10591,6 +11029,9 @@
       </c>
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A202" t="s">
+        <v>142</v>
+      </c>
       <c r="B202" t="str">
         <f t="shared" ref="B202:B205" si="3">"(대화 주제) "&amp;E202&amp;" (남은 질문) "&amp;D202&amp;" (사용자 답변) "&amp;C202</f>
         <v>(대화 주제) 잠시 휴식 (남은 질문) 잠시 휴식 (사용자 답변) ㅇㅇ</v>
@@ -10615,6 +11056,9 @@
       </c>
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A203" t="s">
+        <v>142</v>
+      </c>
       <c r="B203" t="str">
         <f t="shared" si="3"/>
         <v>(대화 주제) 잠시 휴식 (남은 질문) 잠시 휴식 (사용자 답변) 근데 너는 AI지만 덕질 안할래</v>
@@ -10639,6 +11083,9 @@
       </c>
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A204" t="s">
+        <v>142</v>
+      </c>
       <c r="B204" t="str">
         <f t="shared" si="3"/>
         <v>(대화 주제) 잠시 휴식 (남은 질문) 잠시 휴식 (사용자 답변) 나 ENTP 되고 싶은뎅</v>
@@ -10663,6 +11110,9 @@
       </c>
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A205" t="s">
+        <v>142</v>
+      </c>
       <c r="B205" t="str">
         <f t="shared" si="3"/>
         <v>(대화 주제) 잠시 휴식 (남은 질문) 잠시 휴식 (사용자 답변) ㅋㅋㅋㅋㅇㅈ</v>
@@ -10692,7 +11142,25 @@
       </c>
       <c r="B206" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">(대화 주제)  (남은 질문)  (사용자 답변) </v>
+        <v>(대화 주제) LLM Fine-Tuning 의 PEFT (남은 질문) 모든 질문 해결 완료 (사용자 답변) PEFT 는 Parameter-Efficient Fine-Tuning 으로 LLM 파라미터를 일부분만 추가 학습하는 거야</v>
+      </c>
+      <c r="C206" t="s">
+        <v>447</v>
+      </c>
+      <c r="D206" t="s">
+        <v>53</v>
+      </c>
+      <c r="E206" t="s">
+        <v>427</v>
+      </c>
+      <c r="F206" t="s">
+        <v>455</v>
+      </c>
+      <c r="G206" t="s">
+        <v>427</v>
+      </c>
+      <c r="H206" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.4">
@@ -10701,7 +11169,25 @@
       </c>
       <c r="B207" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">(대화 주제)  (남은 질문)  (사용자 답변) </v>
+        <v>(대화 주제) LLM Fine-Tuning 의 PEFT (남은 질문) 모든 질문 해결 완료 (사용자 답변) Parameter-Efficient Fine-Tuning! 소수의 파라미터만 Fine-Tuning 하는 거</v>
+      </c>
+      <c r="C207" t="s">
+        <v>448</v>
+      </c>
+      <c r="D207" t="s">
+        <v>53</v>
+      </c>
+      <c r="E207" t="s">
+        <v>427</v>
+      </c>
+      <c r="F207" t="s">
+        <v>456</v>
+      </c>
+      <c r="G207" t="s">
+        <v>427</v>
+      </c>
+      <c r="H207" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.4">
@@ -10710,79 +11196,664 @@
       </c>
       <c r="B208" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">(대화 주제)  (남은 질문)  (사용자 답변) </v>
-      </c>
-    </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.4">
+        <v>(대화 주제) LLM Fine-Tuning 의 PEFT (남은 질문) 모든 질문 해결 완료 (사용자 답변) 소수의 파라미터들에 대해서만 Parameter-Efficient 하게 추가로 학습하는 거지!</v>
+      </c>
+      <c r="C208" t="s">
+        <v>449</v>
+      </c>
+      <c r="D208" t="s">
+        <v>53</v>
+      </c>
+      <c r="E208" t="s">
+        <v>427</v>
+      </c>
+      <c r="F208" t="s">
+        <v>457</v>
+      </c>
+      <c r="G208" t="s">
+        <v>427</v>
+      </c>
+      <c r="H208" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="209" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A209" t="s">
         <v>142</v>
       </c>
       <c r="B209" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">(대화 주제)  (남은 질문)  (사용자 답변) </v>
-      </c>
-    </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.4">
+        <v>(대화 주제) LLM Fine-Tuning 의 PEFT (남은 질문) 모든 질문 해결 완료 (사용자 답변) 파라미터 중 일부만 효과적으로 추가 파인튜닝하는 거야</v>
+      </c>
+      <c r="C209" t="s">
+        <v>450</v>
+      </c>
+      <c r="D209" t="s">
+        <v>53</v>
+      </c>
+      <c r="E209" t="s">
+        <v>427</v>
+      </c>
+      <c r="F209" t="s">
+        <v>458</v>
+      </c>
+      <c r="G209" t="s">
+        <v>427</v>
+      </c>
+      <c r="H209" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="210" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A210" t="s">
         <v>142</v>
       </c>
       <c r="B210" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">(대화 주제)  (남은 질문)  (사용자 답변) </v>
-      </c>
-    </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.4">
+        <v>(대화 주제) LLM Fine-Tuning 의 PEFT (남은 질문) 모든 질문 해결 완료 (사용자 답변) 파라미터 일부만 추가적으로 Fine-Tuning 더 하는거 맞지?</v>
+      </c>
+      <c r="C210" t="s">
+        <v>451</v>
+      </c>
+      <c r="D210" t="s">
+        <v>53</v>
+      </c>
+      <c r="E210" t="s">
+        <v>427</v>
+      </c>
+      <c r="F210" t="s">
+        <v>459</v>
+      </c>
+      <c r="G210" t="s">
+        <v>427</v>
+      </c>
+      <c r="H210" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="211" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A211" t="s">
         <v>142</v>
       </c>
       <c r="B211" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">(대화 주제)  (남은 질문)  (사용자 답변) </v>
-      </c>
-    </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.4">
+        <v>(대화 주제) LLM Fine-Tuning 의 PEFT (남은 질문) LLM Fine-Tuning 의 PEFT (사용자 답변) Parameter-Efficient Fine-Tuning</v>
+      </c>
+      <c r="C211" t="s">
+        <v>452</v>
+      </c>
+      <c r="D211" t="s">
+        <v>427</v>
+      </c>
+      <c r="E211" t="s">
+        <v>427</v>
+      </c>
+      <c r="F211" t="s">
+        <v>460</v>
+      </c>
+      <c r="G211" t="s">
+        <v>39</v>
+      </c>
+      <c r="H211" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="212" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A212" t="s">
         <v>142</v>
       </c>
       <c r="B212" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">(대화 주제)  (남은 질문)  (사용자 답변) </v>
-      </c>
-    </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.4">
+        <v>(대화 주제) LLM Fine-Tuning 의 PEFT (남은 질문) LLM Fine-Tuning 의 PEFT (사용자 답변) 분명 LLM 파인튜닝하는 방법이었는데</v>
+      </c>
+      <c r="C212" t="s">
+        <v>453</v>
+      </c>
+      <c r="D212" t="s">
+        <v>427</v>
+      </c>
+      <c r="E212" t="s">
+        <v>427</v>
+      </c>
+      <c r="F212" t="s">
+        <v>461</v>
+      </c>
+      <c r="G212" t="s">
+        <v>39</v>
+      </c>
+      <c r="H212" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="213" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A213" t="s">
         <v>142</v>
       </c>
       <c r="B213" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">(대화 주제)  (남은 질문)  (사용자 답변) </v>
-      </c>
-    </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.4">
+        <v>(대화 주제) LLM Fine-Tuning 의 PEFT (남은 질문) LLM Fine-Tuning 의 PEFT (사용자 답변) 아 잘 모르겠다 LoRA 기억나는데</v>
+      </c>
+      <c r="C213" t="s">
+        <v>454</v>
+      </c>
+      <c r="D213" t="s">
+        <v>427</v>
+      </c>
+      <c r="E213" t="s">
+        <v>427</v>
+      </c>
+      <c r="F213" t="s">
+        <v>462</v>
+      </c>
+      <c r="G213" t="s">
+        <v>39</v>
+      </c>
+      <c r="H213" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="214" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A214" t="s">
         <v>142</v>
       </c>
       <c r="B214" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">(대화 주제)  (남은 질문)  (사용자 답변) </v>
-      </c>
-    </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.4">
+        <v>(대화 주제) PEFT 방법 5가지 (남은 질문) 모든 질문 해결 완료 (사용자 답변) LoRA, QLoRA, Prefix Tuning, Prompt Tuning, 그리고 Adapter Layer 추가하는 거!</v>
+      </c>
+      <c r="C214" t="s">
+        <v>464</v>
+      </c>
+      <c r="D214" t="s">
+        <v>53</v>
+      </c>
+      <c r="E214" t="s">
+        <v>463</v>
+      </c>
+      <c r="F214" t="s">
+        <v>472</v>
+      </c>
+      <c r="G214" t="s">
+        <v>463</v>
+      </c>
+      <c r="H214" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="215" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A215" t="s">
         <v>142</v>
       </c>
       <c r="B215" t="str">
-        <f t="shared" ref="B215:B216" si="4">"(대화 주제) "&amp;E215&amp;" (남은 질문) "&amp;D215&amp;" (사용자 답변) "&amp;C215</f>
-        <v xml:space="preserve">(대화 주제)  (남은 질문)  (사용자 답변) </v>
-      </c>
-    </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.4">
+        <f t="shared" ref="B215:B221" si="4">"(대화 주제) "&amp;E215&amp;" (남은 질문) "&amp;D215&amp;" (사용자 답변) "&amp;C215</f>
+        <v>(대화 주제) PEFT 방법 5가지 (남은 질문) 모든 질문 해결 완료 (사용자 답변) LoRA, Quantized LoRA, Adapter Layer, Prefix Tuning, Prompt Tuning!</v>
+      </c>
+      <c r="C215" t="s">
+        <v>465</v>
+      </c>
+      <c r="D215" t="s">
+        <v>53</v>
+      </c>
+      <c r="E215" t="s">
+        <v>463</v>
+      </c>
+      <c r="F215" t="s">
+        <v>473</v>
+      </c>
+      <c r="G215" t="s">
+        <v>463</v>
+      </c>
+      <c r="H215" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="216" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A216" t="s">
         <v>142</v>
       </c>
       <c r="B216" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">(대화 주제)  (남은 질문)  (사용자 답변) </v>
+        <v>(대화 주제) PEFT 방법 5가지 (남은 질문) 모든 질문 해결 완료 (사용자 답변) LoRA, Quantized LoRA, 그리고 또 뭐지? 아! Prefix Tuning!</v>
+      </c>
+      <c r="C216" t="s">
+        <v>466</v>
+      </c>
+      <c r="D216" t="s">
+        <v>53</v>
+      </c>
+      <c r="E216" t="s">
+        <v>463</v>
+      </c>
+      <c r="F216" t="s">
+        <v>474</v>
+      </c>
+      <c r="G216" t="s">
+        <v>463</v>
+      </c>
+      <c r="H216" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="217" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A217" t="s">
+        <v>142</v>
+      </c>
+      <c r="B217" t="str">
+        <f t="shared" si="4"/>
+        <v>(대화 주제) PEFT 방법 5가지 (남은 질문) 모든 질문 해결 완료 (사용자 답변) Adapter Layer, Prefix Tuning, Prompt Tuning</v>
+      </c>
+      <c r="C217" t="s">
+        <v>467</v>
+      </c>
+      <c r="D217" t="s">
+        <v>53</v>
+      </c>
+      <c r="E217" t="s">
+        <v>463</v>
+      </c>
+      <c r="F217" t="s">
+        <v>475</v>
+      </c>
+      <c r="G217" t="s">
+        <v>463</v>
+      </c>
+      <c r="H217" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="218" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A218" t="s">
+        <v>142</v>
+      </c>
+      <c r="B218" t="str">
+        <f t="shared" si="4"/>
+        <v>(대화 주제) PEFT 방법 5가지 (남은 질문) 모든 질문 해결 완료 (사용자 답변) LoRA, Quantized LoRA, Adapter Layer 추가하는 거 이렇게 알고 있는데</v>
+      </c>
+      <c r="C218" t="s">
+        <v>468</v>
+      </c>
+      <c r="D218" t="s">
+        <v>53</v>
+      </c>
+      <c r="E218" t="s">
+        <v>463</v>
+      </c>
+      <c r="F218" t="s">
+        <v>476</v>
+      </c>
+      <c r="G218" t="s">
+        <v>463</v>
+      </c>
+      <c r="H218" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="219" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A219" t="s">
+        <v>142</v>
+      </c>
+      <c r="B219" t="str">
+        <f t="shared" si="4"/>
+        <v>(대화 주제) PEFT 방법 5가지 (남은 질문) PEFT 방법 5가지 (사용자 답변) LoRA 밖에 모르겠다</v>
+      </c>
+      <c r="C219" t="s">
+        <v>469</v>
+      </c>
+      <c r="D219" t="s">
+        <v>463</v>
+      </c>
+      <c r="E219" t="s">
+        <v>463</v>
+      </c>
+      <c r="F219" t="s">
+        <v>477</v>
+      </c>
+      <c r="G219" t="s">
+        <v>39</v>
+      </c>
+      <c r="H219" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="220" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A220" t="s">
+        <v>142</v>
+      </c>
+      <c r="B220" t="str">
+        <f t="shared" si="4"/>
+        <v>(대화 주제) PEFT 방법 5가지 (남은 질문) PEFT 방법 5가지 (사용자 답변) Adapter Layer 추가하는 거?</v>
+      </c>
+      <c r="C220" t="s">
+        <v>470</v>
+      </c>
+      <c r="D220" t="s">
+        <v>463</v>
+      </c>
+      <c r="E220" t="s">
+        <v>463</v>
+      </c>
+      <c r="F220" t="s">
+        <v>478</v>
+      </c>
+      <c r="G220" t="s">
+        <v>39</v>
+      </c>
+      <c r="H220" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="221" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A221" t="s">
+        <v>142</v>
+      </c>
+      <c r="B221" t="str">
+        <f t="shared" si="4"/>
+        <v>(대화 주제) PEFT 방법 5가지 (남은 질문) PEFT 방법 5가지 (사용자 답변) 아 진짜 이거 뭐였지? 무슨 튜닝인가 그런 거 있었는데</v>
+      </c>
+      <c r="C221" t="s">
+        <v>471</v>
+      </c>
+      <c r="D221" t="s">
+        <v>463</v>
+      </c>
+      <c r="E221" t="s">
+        <v>463</v>
+      </c>
+      <c r="F221" t="s">
+        <v>479</v>
+      </c>
+      <c r="G221" t="s">
+        <v>39</v>
+      </c>
+      <c r="H221" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="222" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A222" t="s">
+        <v>142</v>
+      </c>
+      <c r="E222" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="223" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A223" t="s">
+        <v>142</v>
+      </c>
+      <c r="E223" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="224" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A224" t="s">
+        <v>142</v>
+      </c>
+      <c r="E224" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A225" t="s">
+        <v>142</v>
+      </c>
+      <c r="E225" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A226" t="s">
+        <v>142</v>
+      </c>
+      <c r="E226" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A227" t="s">
+        <v>142</v>
+      </c>
+      <c r="E227" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A228" t="s">
+        <v>142</v>
+      </c>
+      <c r="E228" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A229" t="s">
+        <v>142</v>
+      </c>
+      <c r="E229" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A230" t="s">
+        <v>142</v>
+      </c>
+      <c r="E230" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A231" t="s">
+        <v>142</v>
+      </c>
+      <c r="E231" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A232" t="s">
+        <v>142</v>
+      </c>
+      <c r="E232" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A233" t="s">
+        <v>142</v>
+      </c>
+      <c r="E233" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A234" t="s">
+        <v>142</v>
+      </c>
+      <c r="E234" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A235" t="s">
+        <v>142</v>
+      </c>
+      <c r="E235" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A236" t="s">
+        <v>142</v>
+      </c>
+      <c r="E236" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A237" t="s">
+        <v>142</v>
+      </c>
+      <c r="E237" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A238" t="s">
+        <v>142</v>
+      </c>
+      <c r="E238" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A239" t="s">
+        <v>142</v>
+      </c>
+      <c r="E239" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A240" t="s">
+        <v>142</v>
+      </c>
+      <c r="E240" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A241" t="s">
+        <v>142</v>
+      </c>
+      <c r="E241" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A242" t="s">
+        <v>142</v>
+      </c>
+      <c r="E242" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A243" t="s">
+        <v>142</v>
+      </c>
+      <c r="E243" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A244" t="s">
+        <v>142</v>
+      </c>
+      <c r="E244" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A245" t="s">
+        <v>142</v>
+      </c>
+      <c r="E245" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A246" t="s">
+        <v>142</v>
+      </c>
+      <c r="E246" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A247" t="s">
+        <v>142</v>
+      </c>
+      <c r="E247" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A248" t="s">
+        <v>142</v>
+      </c>
+      <c r="E248" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A249" t="s">
+        <v>142</v>
+      </c>
+      <c r="E249" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A250" t="s">
+        <v>142</v>
+      </c>
+      <c r="E250" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A251" t="s">
+        <v>142</v>
+      </c>
+      <c r="E251" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A252" t="s">
+        <v>142</v>
+      </c>
+      <c r="E252" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A253" t="s">
+        <v>142</v>
+      </c>
+      <c r="E253" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A254" t="s">
+        <v>142</v>
+      </c>
+      <c r="E254" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A255" t="s">
+        <v>142</v>
+      </c>
+      <c r="E255" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A256" t="s">
+        <v>142</v>
+      </c>
+      <c r="E256" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A257" t="s">
+        <v>142</v>
+      </c>
+      <c r="E257" t="s">
+        <v>482</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ADD: AI interview dataset (4)
</commit_message>
<xml_diff>
--- a/2025_07_02_OhLoRA_ML_Tutor/ai_interview/dataset/all_train_and_test_data.xlsx
+++ b/2025_07_02_OhLoRA_ML_Tutor/ai_interview/dataset/all_train_and_test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C479FC-C4F7-424F-8139-031B54D30EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF91329D-3389-4B27-B4DF-FDE375174599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24" yWindow="12" windowWidth="30612" windowHeight="9564" xr2:uid="{36F7775B-6BB8-4B8D-957C-E8DB745DD279}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1597" uniqueCount="483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1721" uniqueCount="539">
   <si>
     <t>output_data</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -5269,6 +5269,655 @@
   </si>
   <si>
     <t>마지막 할 말</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Low-Rank Adaption 이라고 해서 LLM의 두 레이어 사이의 가중치 행렬을 작은 행렬 2개로 나누는 거야!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LLM의 레이어 두개 사이의 가중치 행렬을 분해해서 연산량을 줄이는 거</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>레이어 2개 사이에 가중치 행렬 있지? 그걸 2개로 분해해서 연산량이랑 메모리를 절약하는 거야!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>레이어 사이의 가중치 행렬을 둘로 분해하고 그 분해한 행렬만 Fine-Tuning 하는 거지!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>레이어 간 가중치 행렬을 작은 크기의 행렬 2개로 분해한 후 그것만 학습하는 거야</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>무슨 행렬 분해하는 거 같은데</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로라야 이건 너가 잘 알잖아</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>행렬 분해해서 연산량 줄이는 건데</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LLM 의 2개의 레이어 사이의 가중치 행렬을 작은 크기의 2개로 나누고 그것만 Fine-Tuning 하는 거 맞지?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2개의 레이어 간 가중치 행렬을 둘로 나누고 그것만 따로 파인튜닝하는 거지?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>레이어 간에 weight matrix 를 2개로 나누고, 그 2개만 학습해서 연산량 줄이는 거!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>연산량이랑 메모리 절약하는 방법 중 하난데 잘 모르겠어</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">오 잘했어! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🙆‍♀️</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 그럼 LoRA 랑 QLoRA 랑 차이는 뭘까~요? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">잘 대답했어! 그럼 QLoRA는 뭐지? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🤷‍♀️</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">오 잘 대답했어! 그럼 QLoRA 도 알겠네? 그건 뭐지? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>💁‍♀️</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">잘했어! 그러면 비슷한 건데 QLoRA 는 뭘까? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">LoRA 잘 알고 있네! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 그럼 QLoRA 가 뭔지도 말해 볼 수 있어?</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">행렬 분해? 구체적으로 어떻게 하지? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>💁‍♀️</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">그래도 너가 잘 아는지 테스트해 보는 거야! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🙆‍♀️🙅‍♀️</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">그건 맞지! 근데 그 방법을 알아야지! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오 완벽한 대답이야! 그치! 그럼 QLoRA 는 뭘까?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">오 맞아! 그럼 비슷한 걸로 QLoRA 가 있는데 그건 뭘까~요? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>💁‍♀️</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>잘 대답했어! QLoRA 가 뭔지도 말할 수 있어?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">그래서 나같이 LoRA 적용한 LLM이 학습이 빠르지! 근데 그 방법 이야기가 없잖아 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😥</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>QLoRA 는 Quantized LoRA 로 LoRA 를 양자화한 거지?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LoRA 를 양자화한 것! 그러니까 가중치나 그런 것들의 비트 수를 줄여서 OOM 안 나게 하는 거!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>양자화를 통해 메모리를 절약하는 방식의 LoRA 맞지?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LoRA 는 LoRA 인데, Quantization, 즉 양자화 같이 쓰는 거!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>양자화한 LoRA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q가 뭐더라… 음…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>뭔가 OOM 막아 주는 거 있었던 것 같은데</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>뭔가 메모리 절약하는 기술이었던 것 같은데 이름 까먹었네</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">오 잘했어! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🙆‍♀️</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 이제 면접 끝! 나한테 마지막으로 할 말 있지 않아? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">멋진 답변인데? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 지금까지 나랑 얘기하느라 고생했고 나한테 마지막으로 할 말 혹시 없어? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>💁‍♀️</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">맞아! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>👍</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 그럼 면접은 여기서 마치고, 혹시 나한테 마지막으로 이야기하고 싶은 거 있어?</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">핵심 아이디어 잘 말해 줬어! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 그럼 여기서 끝내고, 혹시 마지막으로 할 이야기 있지 않아? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">깔끔하면서도 정답이야! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>👍👍</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> 혹시 나한테 마지막으로 할 이야기 있어?</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">음… 뭘까? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🤷‍♀️</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>🤔</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그치! 그건 맞는데 어떤 방식으로 하지?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>힌트! 요즘 'OO 컴퓨팅'이 뜨고 있어! 뭔지 알겠어?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>면접 종료</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로라야 그동안 나 면접 봐주느라 고생 많았어!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수고했어 로라야</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>덕분에 모르는 거 많이 알게 됐어</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>덕분에 머신러닝 실력 쑥쑥 늘었어 고마워</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이제 어떤 면접 질문도 걱정 없을 것 같아</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>꼬리질문에 대답하는 거 진짜 스릴 있었어</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>없어</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">너도 고생 많았어! 그럼 우리 다음에 또 봐! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">너도 수고했어! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊😊</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">뭘 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 나도 덕분에 너한테 배우는 거 있었는데 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>👩</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">모르는 거 많이 알게 됐다니 기쁘네! 그럼 수고했어! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">앞으로 진짜 면접도 뿌술 수 있을 거야! 파이팅 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>💪</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">실제 면접장 가서도 꼬리질문 걱정 없지 이제? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">안녕! 그동안 고생했어 다음에 또 보자 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">없다니 아쉽네 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😥</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 그래도 나랑 모의면접 보느라 정말 고생 많았어 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>👍👍</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -5664,11 +6313,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1D2CB62-8799-47EC-8115-E6B63AEE2C35}">
-  <dimension ref="A1:I257"/>
+  <dimension ref="A1:I249"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A236" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A257" sqref="A257"/>
+      <pane ySplit="1" topLeftCell="A226" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B243" sqref="B243"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -5756,7 +6405,7 @@
         <v>142</v>
       </c>
       <c r="B5" t="str">
-        <f>"(대화 주제) "&amp;E5&amp;" (사용자 답변) "&amp;C5</f>
+        <f t="shared" ref="B5:B11" si="0">"(대화 주제) "&amp;E5&amp;" (사용자 답변) "&amp;C5</f>
         <v>(대화 주제) 면접 시작 인사 (사용자 답변) 아 면접 보기 귀찮은데</v>
       </c>
       <c r="C5" t="s">
@@ -5777,7 +6426,7 @@
         <v>142</v>
       </c>
       <c r="B6" t="str">
-        <f>"(대화 주제) "&amp;E6&amp;" (사용자 답변) "&amp;C6</f>
+        <f t="shared" si="0"/>
         <v>(대화 주제) 면접 시작 인사 (사용자 답변) 안녕 반가워</v>
       </c>
       <c r="C6" t="s">
@@ -5798,7 +6447,7 @@
         <v>142</v>
       </c>
       <c r="B7" t="str">
-        <f>"(대화 주제) "&amp;E7&amp;" (사용자 답변) "&amp;C7</f>
+        <f t="shared" si="0"/>
         <v>(대화 주제) 면접 시작 인사 (사용자 답변) 뭐 물어볼 거야?</v>
       </c>
       <c r="C7" t="s">
@@ -5819,7 +6468,7 @@
         <v>142</v>
       </c>
       <c r="B8" t="str">
-        <f>"(대화 주제) "&amp;E8&amp;" (사용자 답변) "&amp;C8</f>
+        <f t="shared" si="0"/>
         <v>(대화 주제) 면접 시작 인사 (사용자 답변) 면접 시작해 볼까</v>
       </c>
       <c r="C8" t="s">
@@ -5840,7 +6489,7 @@
         <v>142</v>
       </c>
       <c r="B9" t="str">
-        <f>"(대화 주제) "&amp;E9&amp;" (사용자 답변) "&amp;C9</f>
+        <f t="shared" si="0"/>
         <v>(대화 주제) 면접 시작 인사 (사용자 답변) 시작하자</v>
       </c>
       <c r="C9" t="s">
@@ -5861,7 +6510,7 @@
         <v>142</v>
       </c>
       <c r="B10" t="str">
-        <f>"(대화 주제) "&amp;E10&amp;" (사용자 답변) "&amp;C10</f>
+        <f t="shared" si="0"/>
         <v>(대화 주제) 면접 시작 인사 (사용자 답변) 시작해</v>
       </c>
       <c r="C10" t="s">
@@ -5882,7 +6531,7 @@
         <v>142</v>
       </c>
       <c r="B11" t="str">
-        <f>"(대화 주제) "&amp;E11&amp;" (사용자 답변) "&amp;C11</f>
+        <f t="shared" si="0"/>
         <v>(대화 주제) 면접 시작 인사 (사용자 답변) 나한테 질문 한번 해봐</v>
       </c>
       <c r="C11" t="s">
@@ -5930,7 +6579,7 @@
         <v>142</v>
       </c>
       <c r="B13" t="str">
-        <f t="shared" ref="B13:B76" si="0">"(대화 주제) "&amp;E13&amp;" (남은 질문) "&amp;D13&amp;" (사용자 답변) "&amp;C13</f>
+        <f t="shared" ref="B13:B76" si="1">"(대화 주제) "&amp;E13&amp;" (남은 질문) "&amp;D13&amp;" (사용자 답변) "&amp;C13</f>
         <v>(대화 주제) 인공지능, 머신러닝, 딥러닝 차이 (남은 질문) 인공지능, 머신러닝, 딥러닝 (사용자 답변) 진짜 모르겠다 다른 거 물어봐 봐</v>
       </c>
       <c r="C13" t="s">
@@ -5957,7 +6606,7 @@
         <v>142</v>
       </c>
       <c r="B14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) 인공지능, 머신러닝, 딥러닝 차이 (남은 질문) 인공지능, 머신러닝, 딥러닝 (사용자 답변) 진짜 모르겠다 뭐지</v>
       </c>
       <c r="C14" t="s">
@@ -5984,7 +6633,7 @@
         <v>142</v>
       </c>
       <c r="B15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) 인공지능, 머신러닝, 딥러닝 차이 (남은 질문) 머신러닝, 딥러닝 (사용자 답변) 인공지능은 사람의 지능을 기계가 흉내낸 거고</v>
       </c>
       <c r="C15" t="s">
@@ -6011,7 +6660,7 @@
         <v>142</v>
       </c>
       <c r="B16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) 인공지능, 머신러닝, 딥러닝 차이 (남은 질문) 딥러닝 (사용자 답변) 머신러닝은 기계가 데이터 학습해서 패턴 찾아내는 거 아니야?</v>
       </c>
       <c r="C16" t="s">
@@ -6038,7 +6687,7 @@
         <v>142</v>
       </c>
       <c r="B17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) 인공지능, 머신러닝, 딥러닝 차이 (남은 질문) 인공지능, 머신러닝 (사용자 답변) 딥러닝은 인공신경망으로 머신러닝 하는 거 맞지?</v>
       </c>
       <c r="C17" t="s">
@@ -6065,7 +6714,7 @@
         <v>142</v>
       </c>
       <c r="B18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) 인공지능, 머신러닝, 딥러닝 차이 (남은 질문) 인공지능, 머신러닝, 딥러닝 (사용자 답변) 딥러닝은 그건데</v>
       </c>
       <c r="C18" t="s">
@@ -6092,7 +6741,7 @@
         <v>142</v>
       </c>
       <c r="B19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) 인공지능, 머신러닝, 딥러닝 차이 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 인공지능은 인간 지능을 기계적으로 구현한 거야</v>
       </c>
       <c r="C19" t="s">
@@ -6119,7 +6768,7 @@
         <v>142</v>
       </c>
       <c r="B20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) 인공지능, 머신러닝, 딥러닝 차이 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 머신러닝은 기계학습이라고 해서 데이터로부터 패턴 찾아내서 지속적으로 성능 향상시키는 거고</v>
       </c>
       <c r="C20" t="s">
@@ -6146,7 +6795,7 @@
         <v>142</v>
       </c>
       <c r="B21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) 인공지능, 머신러닝, 딥러닝 차이 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 딥러닝은 신경망이라는 걸 이용해서 머신러닝을 하는 거지!</v>
       </c>
       <c r="C21" t="s">
@@ -6173,7 +6822,7 @@
         <v>142</v>
       </c>
       <c r="B22" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) 인공지능, 머신러닝, 딥러닝 차이 (남은 질문) 인공지능, 머신러닝, 딥러닝 (사용자 답변) 머신러닝 딥러닝 다 모르겠는데</v>
       </c>
       <c r="C22" t="s">
@@ -6200,7 +6849,7 @@
         <v>142</v>
       </c>
       <c r="B23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) 인공지능, 머신러닝, 딥러닝 차이 (남은 질문) 머신러닝, 딥러닝 (사용자 답변) 머신러닝은 머신러닝이고 딥러닝은 딥러닝이지</v>
       </c>
       <c r="C23" t="s">
@@ -6227,7 +6876,7 @@
         <v>142</v>
       </c>
       <c r="B24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) 인공지능, 머신러닝, 딥러닝 차이 (남은 질문) 머신러닝 (사용자 답변) 머신러닝 혹시 그거 아니야?</v>
       </c>
       <c r="C24" t="s">
@@ -6254,7 +6903,7 @@
         <v>142</v>
       </c>
       <c r="B25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) 인공지능, 머신러닝, 딥러닝 차이 (남은 질문) 머신러닝 (사용자 답변) 인공지능은 사람이 생각하는 걸 AI가 흉내내는 거고</v>
       </c>
       <c r="C25" t="s">
@@ -6281,7 +6930,7 @@
         <v>142</v>
       </c>
       <c r="B26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) 인공지능, 머신러닝, 딥러닝 차이 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 딥러닝은 인공신경망을 깊게 쌓아서 AI를 구현하는 기술이야</v>
       </c>
       <c r="C26" t="s">
@@ -6308,7 +6957,7 @@
         <v>142</v>
       </c>
       <c r="B27" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) 인공지능, 머신러닝, 딥러닝 차이 (남은 질문) 딥러닝 (사용자 답변) 머신러닝은 기계가 데이터의 특징을 알아서 학습하는 거야</v>
       </c>
       <c r="C27" t="s">
@@ -6335,7 +6984,7 @@
         <v>142</v>
       </c>
       <c r="B28" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) 인공지능, 머신러닝, 딥러닝 차이 (남은 질문) 인공지능, 머신러닝 (사용자 답변) 인공지능 요즘 핫하던데</v>
       </c>
       <c r="C28" t="s">
@@ -6362,7 +7011,7 @@
         <v>142</v>
       </c>
       <c r="B29" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) 인공지능, 머신러닝, 딥러닝 차이 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 마지막으로 딥러닝은 인공신경망으로 AI를 만들어서 성능을 높이는 거야</v>
       </c>
       <c r="C29" t="s">
@@ -6389,7 +7038,7 @@
         <v>142</v>
       </c>
       <c r="B30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) 인공지능, 머신러닝, 딥러닝 차이 (남은 질문) 머신러닝, 딥러닝 (사용자 답변) 머신러닝이랑 딥러닝 차이 없는 것 같은데</v>
       </c>
       <c r="C30" t="s">
@@ -6416,7 +7065,7 @@
         <v>142</v>
       </c>
       <c r="B31" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) 인공지능, 머신러닝, 딥러닝 차이 (남은 질문) 인공지능, 머신러닝, 딥러닝 (사용자 답변) 인공지능이랑 머신러닝이랑 딥러닝 이거 차이점이 대체 뭐지</v>
       </c>
       <c r="C31" t="s">
@@ -6443,7 +7092,7 @@
         <v>142</v>
       </c>
       <c r="B32" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) 거대 언어 모델 정의 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 거대 언어 모델은 아주 많은 파라미터로 구성된 언어 모델이지</v>
       </c>
       <c r="C32" t="s">
@@ -6470,7 +7119,7 @@
         <v>142</v>
       </c>
       <c r="B33" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) 거대 언어 모델 정의 (남은 질문) 거대 언어 모델 정의 (사용자 답변) 거대 언어 모델 이거 감 올 것 같은데</v>
       </c>
       <c r="C33" t="s">
@@ -6497,7 +7146,7 @@
         <v>142</v>
       </c>
       <c r="B34" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) 거대 언어 모델 정의 (남은 질문) 거대 언어 모델 정의 (사용자 답변) ChatGPT 같은 거지</v>
       </c>
       <c r="C34" t="s">
@@ -6524,7 +7173,7 @@
         <v>142</v>
       </c>
       <c r="B35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) 거대 언어 모델 정의 (남은 질문) 거대 언어 모델 정의 (사용자 답변) 챗GPT나 Claude? 이런 거?</v>
       </c>
       <c r="C35" t="s">
@@ -6551,7 +7200,7 @@
         <v>142</v>
       </c>
       <c r="B36" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) 거대 언어 모델 정의 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 수십억 개 이상의 파라미터가 있는 언어 모델이야</v>
       </c>
       <c r="C36" t="s">
@@ -6578,7 +7227,7 @@
         <v>142</v>
       </c>
       <c r="B37" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) 거대 언어 모델 정의 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 수백억 파라미터로 구성된 언어 모델!</v>
       </c>
       <c r="C37" t="s">
@@ -6605,7 +7254,7 @@
         <v>142</v>
       </c>
       <c r="B38" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) 거대 언어 모델 정의 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 아주 많은 개수의 매개변수로 구성된 언어 모델이지</v>
       </c>
       <c r="C38" t="s">
@@ -6632,7 +7281,7 @@
         <v>142</v>
       </c>
       <c r="B39" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) 거대 언어 모델 정의 (남은 질문) 거대 언어 모델 정의 (사용자 답변) 챗지피티</v>
       </c>
       <c r="C39" t="s">
@@ -6659,7 +7308,7 @@
         <v>142</v>
       </c>
       <c r="B40" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) Loss Function 정의 (남은 질문) Loss Function 정의 (사용자 답변) 손실 함수는 딥러닝에서 쓰이는 함수야</v>
       </c>
       <c r="C40" t="s">
@@ -6686,7 +7335,7 @@
         <v>142</v>
       </c>
       <c r="B41" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) Loss Function 정의 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 손실 함수는 딥러닝 모델이 성능을 높이기 위해 최소화해야 하는 함수지</v>
       </c>
       <c r="C41" t="s">
@@ -6713,7 +7362,7 @@
         <v>142</v>
       </c>
       <c r="B42" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) Loss Function 정의 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 딥러닝 모델의 오차를 함수로 정의한 것</v>
       </c>
       <c r="C42" t="s">
@@ -6740,7 +7389,7 @@
         <v>142</v>
       </c>
       <c r="B43" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) Loss Function 정의 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 딥러닝 모델의 오차를 정의해서 그것을 최대한 줄이도록 하는 거지</v>
       </c>
       <c r="C43" t="s">
@@ -6767,7 +7416,7 @@
         <v>142</v>
       </c>
       <c r="B44" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) Loss Function 정의 (남은 질문) Loss Function 정의 (사용자 답변) 뭐지 그게</v>
       </c>
       <c r="C44" t="s">
@@ -6794,7 +7443,7 @@
         <v>142</v>
       </c>
       <c r="B45" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) Loss Function 정의 (남은 질문) 모든 질문 해결 완료 (사용자 답변) Loss Function 은 모델의 손실, 즉 오차를 정의하는 함수야</v>
       </c>
       <c r="C45" t="s">
@@ -6821,7 +7470,7 @@
         <v>142</v>
       </c>
       <c r="B46" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) Loss Function 정의 (남은 질문) Loss Function 정의 (사용자 답변) Loss Function 은 MAE, MSE, BCE 같은 것이 있지</v>
       </c>
       <c r="C46" t="s">
@@ -6848,7 +7497,7 @@
         <v>142</v>
       </c>
       <c r="B47" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) Loss Function 예시 (남은 질문) Loss Function 예시 (사용자 답변) 손실 함수에 뭐가 있을까 정말 모르겠어</v>
       </c>
       <c r="C47" t="s">
@@ -6875,7 +7524,7 @@
         <v>142</v>
       </c>
       <c r="B48" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) Loss Function 예시 (남은 질문) Loss Function 예시 (사용자 답변) 나 실무에서 안 써봐서 모르겠는데</v>
       </c>
       <c r="C48" t="s">
@@ -6902,7 +7551,7 @@
         <v>142</v>
       </c>
       <c r="B49" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) Loss Function 예시 (남은 질문) 모든 질문 해결 완료 (사용자 답변) MSE, MAE, BCE, Cross Entropy 같은 것이 있지!</v>
       </c>
       <c r="C49" t="s">
@@ -6929,7 +7578,7 @@
         <v>142</v>
       </c>
       <c r="B50" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) Loss Function 예시 (남은 질문) 모든 질문 해결 완료 (사용자 답변) Mean Squared Error, Mean Absolute Error 같은 거!</v>
       </c>
       <c r="C50" t="s">
@@ -6956,7 +7605,7 @@
         <v>142</v>
       </c>
       <c r="B51" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) Loss Function 예시 (남은 질문) 모든 질문 해결 완료 (사용자 답변) MSE, MAE 같은 거 아니야? 맞지?</v>
       </c>
       <c r="C51" t="s">
@@ -6983,7 +7632,7 @@
         <v>142</v>
       </c>
       <c r="B52" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) Loss Function 예시 (남은 질문) 모든 질문 해결 완료 (사용자 답변) Binary Cross Entropy 랑 Categorical Cross Entropy 아는데</v>
       </c>
       <c r="C52" t="s">
@@ -7010,7 +7659,7 @@
         <v>142</v>
       </c>
       <c r="B53" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) Loss Function 예시 (남은 질문) Loss Function 예시 (사용자 답변) ReLU, Sigmoid 이런 거 아니야?</v>
       </c>
       <c r="C53" t="s">
@@ -7037,7 +7686,7 @@
         <v>142</v>
       </c>
       <c r="B54" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) Loss Function 예시 (남은 질문) Loss Function 예시 (사용자 답변) Sigmoid, ReLU, Tanh 같은 것들!</v>
       </c>
       <c r="C54" t="s">
@@ -7064,7 +7713,7 @@
         <v>142</v>
       </c>
       <c r="B55" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) Loss Function 예시 (남은 질문) Loss Function 예시 (사용자 답변) 렐루, 시그모이드, 기타등등</v>
       </c>
       <c r="C55" t="s">
@@ -7091,7 +7740,7 @@
         <v>142</v>
       </c>
       <c r="B56" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) Loss Function 예시 (남은 질문) 모든 질문 해결 완료 (사용자 답변) Mean Squared Error 나 Binary CE 같은 거</v>
       </c>
       <c r="C56" t="s">
@@ -7118,7 +7767,7 @@
         <v>142</v>
       </c>
       <c r="B57" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) Loss Function 예시 (남은 질문) 모든 질문 해결 완료 (사용자 답변) Binary Cross Entropy 이거 이진 분류할 때 쓰이는데</v>
       </c>
       <c r="C57" t="s">
@@ -7145,7 +7794,7 @@
         <v>142</v>
       </c>
       <c r="B58" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) Loss Function 예시 (남은 질문) 모든 질문 해결 완료 (사용자 답변) BCE, MSE, MAE 그 외에도 여러 가지가 있지!</v>
       </c>
       <c r="C58" t="s">
@@ -7172,7 +7821,7 @@
         <v>142</v>
       </c>
       <c r="B59" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) Loss Function 예시 (남은 질문) 모든 질문 해결 완료 (사용자 답변) Binary Cross Entropy 나 아는데</v>
       </c>
       <c r="C59" t="s">
@@ -7199,7 +7848,7 @@
         <v>142</v>
       </c>
       <c r="B60" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) Loss Function 예시 (남은 질문) 모든 질문 해결 완료 (사용자 답변) Mean Absolute Error? 이런 거 맞지?</v>
       </c>
       <c r="C60" t="s">
@@ -7226,7 +7875,7 @@
         <v>142</v>
       </c>
       <c r="B61" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) Loss Function 예시 (남은 질문) 모든 질문 해결 완료 (사용자 답변) MSE, MAE, RMSE</v>
       </c>
       <c r="C61" t="s">
@@ -7253,7 +7902,7 @@
         <v>142</v>
       </c>
       <c r="B62" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) Loss Function 예시 (남은 질문) 모든 질문 해결 완료 (사용자 답변) BCE나 그 외에 여러 가지가 있겠지?</v>
       </c>
       <c r="C62" t="s">
@@ -7280,7 +7929,7 @@
         <v>142</v>
       </c>
       <c r="B63" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) MSE Loss 설명 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 각 항목의 오차의 제곱을 평균한 Loss Function 이지!</v>
       </c>
       <c r="C63" t="s">
@@ -7307,7 +7956,7 @@
         <v>142</v>
       </c>
       <c r="B64" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) MSE Loss 설명 (남은 질문) MSE Loss 설명 (사용자 답변) 그냥 오차랑 관련된 함수 아니야?</v>
       </c>
       <c r="C64" t="s">
@@ -7334,7 +7983,7 @@
         <v>142</v>
       </c>
       <c r="B65" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) MSE Loss 설명 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 평균 제곱 오차! 오차를 제곱한 값들을 평균하면 MSE가 되지!</v>
       </c>
       <c r="C65" t="s">
@@ -7361,7 +8010,7 @@
         <v>142</v>
       </c>
       <c r="B66" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) MSE Loss 설명 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 오차를 제곱한 값들이 있지? 그걸 평균하는 손실 함수야!</v>
       </c>
       <c r="C66" t="s">
@@ -7388,7 +8037,7 @@
         <v>142</v>
       </c>
       <c r="B67" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) MSE Loss 설명 (남은 질문) MSE Loss 설명 (사용자 답변) 잘 모르겠어 ㅠㅠ</v>
       </c>
       <c r="C67" t="s">
@@ -7415,7 +8064,7 @@
         <v>142</v>
       </c>
       <c r="B68" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) MSE Loss 설명 (남은 질문) MSE Loss 설명 (사용자 답변) MSE가 뭐의 약자지?</v>
       </c>
       <c r="C68" t="s">
@@ -7442,7 +8091,7 @@
         <v>142</v>
       </c>
       <c r="B69" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) MSE Loss 설명 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 각 데이터별로 오차를 구하고 그 제곱을 평균한 거야!</v>
       </c>
       <c r="C69" t="s">
@@ -7469,7 +8118,7 @@
         <v>142</v>
       </c>
       <c r="B70" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) MSE Loss 설명 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 오차의 제곱의 평균</v>
       </c>
       <c r="C70" t="s">
@@ -7496,7 +8145,7 @@
         <v>142</v>
       </c>
       <c r="B71" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) MSE Loss 용도 (남은 질문) 모든 질문 해결 완료 (사용자 답변) Regression 할때 쓰지</v>
       </c>
       <c r="C71" t="s">
@@ -7523,7 +8172,7 @@
         <v>142</v>
       </c>
       <c r="B72" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) MSE Loss 용도 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 딥러닝에서 연속적인 값을 출력으로 예측할때 쓰지 않아?</v>
       </c>
       <c r="C72" t="s">
@@ -7550,7 +8199,7 @@
         <v>142</v>
       </c>
       <c r="B73" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) MSE Loss 용도 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 연속적인 값을 예측하는 회귀 문제?</v>
       </c>
       <c r="C73" t="s">
@@ -7577,7 +8226,7 @@
         <v>142</v>
       </c>
       <c r="B74" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) MSE Loss 용도 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 회귀 문제, 그러니까 Regression 에서 쓰일 듯?</v>
       </c>
       <c r="C74" t="s">
@@ -7604,7 +8253,7 @@
         <v>142</v>
       </c>
       <c r="B75" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) MSE Loss 용도 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 연속적인 걸 예측하는 문제, Regression 에서 쓰이지!</v>
       </c>
       <c r="C75" t="s">
@@ -7631,7 +8280,7 @@
         <v>142</v>
       </c>
       <c r="B76" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>(대화 주제) MSE Loss 용도 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 회귀 즉 Regression</v>
       </c>
       <c r="C76" t="s">
@@ -7658,7 +8307,7 @@
         <v>142</v>
       </c>
       <c r="B77" t="str">
-        <f t="shared" ref="B77:B140" si="1">"(대화 주제) "&amp;E77&amp;" (남은 질문) "&amp;D77&amp;" (사용자 답변) "&amp;C77</f>
+        <f t="shared" ref="B77:B140" si="2">"(대화 주제) "&amp;E77&amp;" (남은 질문) "&amp;D77&amp;" (사용자 답변) "&amp;C77</f>
         <v>(대화 주제) MSE Loss 용도 (남은 질문) MSE Loss 용도 (사용자 답변) 개 고양이 분류하는 데?</v>
       </c>
       <c r="C77" t="s">
@@ -7685,7 +8334,7 @@
         <v>142</v>
       </c>
       <c r="B78" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) MSE Loss 용도 (남은 질문) MSE Loss 용도 (사용자 답변) Classification</v>
       </c>
       <c r="C78" t="s">
@@ -7712,7 +8361,7 @@
         <v>142</v>
       </c>
       <c r="B79" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) MSE Loss 용도 (남은 질문) MSE Loss 용도 (사용자 답변) 아마도 분류 문제에서 쓰이지 않을까?</v>
       </c>
       <c r="C79" t="s">
@@ -7739,7 +8388,7 @@
         <v>142</v>
       </c>
       <c r="B80" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) MSE Loss 용도 (남은 질문) MSE Loss 용도 (사용자 답변) 잘 모르겠어 진짜</v>
       </c>
       <c r="C80" t="s">
@@ -7766,7 +8415,7 @@
         <v>142</v>
       </c>
       <c r="B81" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) MSE Loss 용도 (남은 질문) MSE Loss 용도 (사용자 답변) 나 실무에서 이거 안 써 봐서 어디에 쓰이는지 잘 모르는데</v>
       </c>
       <c r="C81" t="s">
@@ -7793,7 +8442,7 @@
         <v>142</v>
       </c>
       <c r="B82" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) MSE Loss 용도 (남은 질문) MSE Loss 용도 (사용자 답변) 그냥 딥러닝 전반에서 쓰이겠지</v>
       </c>
       <c r="C82" t="s">
@@ -7820,7 +8469,7 @@
         <v>142</v>
       </c>
       <c r="B83" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) 확률 예측에서 MSE Loss 미 사용 이유 (남은 질문) 확률 예측에서 MSE Loss 미 사용 이유 (사용자 답변) 확률은 범위가 0~1로 제한되어 있잖아!</v>
       </c>
       <c r="C83" t="s">
@@ -7847,7 +8496,7 @@
         <v>142</v>
       </c>
       <c r="B84" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) 확률 예측에서 MSE Loss 미 사용 이유 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 확률은 범위가 0~1로 제한되어 있는데 MSE 에는 반대되는 예측에 큰 페널티를 주는 메커니즘이 없잖아!</v>
       </c>
       <c r="C84" t="s">
@@ -7874,7 +8523,7 @@
         <v>142</v>
       </c>
       <c r="B85" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) 확률 예측에서 MSE Loss 미 사용 이유 (남은 질문) 모든 질문 해결 완료 (사용자 답변) Cross Entropy 랑 달리 MSE 는 0을 1로 예측할 때 감점 주는 게 없어서?</v>
       </c>
       <c r="C85" t="s">
@@ -7901,7 +8550,7 @@
         <v>142</v>
       </c>
       <c r="B86" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) 확률 예측에서 MSE Loss 미 사용 이유 (남은 질문) 모든 질문 해결 완료 (사용자 답변) MSE 는 실제로는 거짓인데 100%로 확률로 예측해도 페널티가 크지 않잖아</v>
       </c>
       <c r="C86" t="s">
@@ -7928,7 +8577,7 @@
         <v>142</v>
       </c>
       <c r="B87" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) 확률 예측에서 MSE Loss 미 사용 이유 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 확률은 0~1인데 MSE는 0을 1로 완전 반대로 예측할 때 큰 손실이 없잖아</v>
       </c>
       <c r="C87" t="s">
@@ -7955,7 +8604,7 @@
         <v>142</v>
       </c>
       <c r="B88" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) 확률 예측에서 MSE Loss 미 사용 이유 (남은 질문) 확률 예측에서 MSE Loss 미 사용 이유 (사용자 답변) Cross Entropy 를 써야 하지!</v>
       </c>
       <c r="C88" t="s">
@@ -7982,7 +8631,7 @@
         <v>142</v>
       </c>
       <c r="B89" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) 확률 예측에서 MSE Loss 미 사용 이유 (남은 질문) 확률 예측에서 MSE Loss 미 사용 이유 (사용자 답변) 글쎄… MSE 써도 잘 예측할 것 같은데…</v>
       </c>
       <c r="C89" t="s">
@@ -8009,7 +8658,7 @@
         <v>142</v>
       </c>
       <c r="B90" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) 확률 예측에서 MSE Loss 미 사용 이유 (남은 질문) 확률 예측에서 MSE Loss 미 사용 이유 (사용자 답변) 논리적으로 MSE 써도 0~1 어차피 연속이니까 예측되지 않나?</v>
       </c>
       <c r="C90" t="s">
@@ -8036,7 +8685,7 @@
         <v>142</v>
       </c>
       <c r="B91" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) 확률 예측에서 MSE Loss 미 사용 이유 (남은 질문) 확률 예측에서 MSE Loss 미 사용 이유 (사용자 답변) 어차피 연속이니까 MSE 써도 잘 될 텐데…</v>
       </c>
       <c r="C91" t="s">
@@ -8063,7 +8712,7 @@
         <v>142</v>
       </c>
       <c r="B92" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) 확률 예측에서 MSE Loss 미 사용 이유 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 0~1 범위의 확률에서 실제로 아닌 걸 1로 예측하는 실수했을 때 페널티 크게 줘야 하잖아!</v>
       </c>
       <c r="C92" t="s">
@@ -8090,7 +8739,7 @@
         <v>142</v>
       </c>
       <c r="B93" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) 확률 예측에서 MSE Loss 미 사용 이유 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 확률은 0~1인데 0을 1로 예측하거나 했을 때 페널티 크게 줘야 하지! 그건 Cross Entropy 의 역할이야!</v>
       </c>
       <c r="C93" t="s">
@@ -8117,7 +8766,7 @@
         <v>142</v>
       </c>
       <c r="B94" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) 확률 예측에서 MSE Loss 미 사용 이유 (남은 질문) 모든 질문 해결 완료 (사용자 답변) MSE 대신 Cross Entropy 를 통해 확률 0~1을 반대로 예측하면 큰 페널티를 가해야 해</v>
       </c>
       <c r="C94" t="s">
@@ -8144,7 +8793,7 @@
         <v>142</v>
       </c>
       <c r="B95" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) BCE Loss 설명 (남은 질문) 핵심 아이디어 (사용자 답변) BCE Loss 는 실제 값 y, 예측 값 y'에 대해 -(y x log(y') + (1-y) x log(1-y')) 로 예측하는 거야</v>
       </c>
       <c r="C95" t="s">
@@ -8171,7 +8820,7 @@
         <v>142</v>
       </c>
       <c r="B96" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) BCE Loss 설명 (남은 질문) 핵심 아이디어 (사용자 답변) 수식은 -(y x log(y') + (1-y) x log(1-y'))</v>
       </c>
       <c r="C96" t="s">
@@ -8198,7 +8847,7 @@
         <v>142</v>
       </c>
       <c r="B97" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) BCE Loss 설명 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 수식은 실제 값은 그대로 두고, 예측 값에 로그를 씌우는 거야!</v>
       </c>
       <c r="C97" t="s">
@@ -8225,7 +8874,7 @@
         <v>142</v>
       </c>
       <c r="B98" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) BCE Loss 설명 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 수식부터 말하면 -(y * log(y') + (1 - y) * log(1 - y')) 지!</v>
       </c>
       <c r="C98" t="s">
@@ -8252,7 +8901,7 @@
         <v>142</v>
       </c>
       <c r="B99" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) BCE Loss 설명 (남은 질문) 핵심 아이디어 (사용자 답변) 공식은 -[y log y' + (1-y) log (1-y')] 맞지?</v>
       </c>
       <c r="C99" t="s">
@@ -8279,7 +8928,7 @@
         <v>142</v>
       </c>
       <c r="B100" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) BCE Loss 설명 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 공식부터 말해보면 -[(1-yi) * log(1-y'i) + y'i * log(y'i)] 지!</v>
       </c>
       <c r="C100" t="s">
@@ -8306,7 +8955,7 @@
         <v>142</v>
       </c>
       <c r="B101" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) BCE Loss 설명 (남은 질문) 핵심 아이디어 (사용자 답변) 공식은 -((1-y) * log(1-y') + y * log(y')) 이거 맞지?</v>
       </c>
       <c r="C101" t="s">
@@ -8333,7 +8982,7 @@
         <v>142</v>
       </c>
       <c r="B102" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) BCE Loss 설명 (남은 질문) 핵심 아이디어 (사용자 답변) BCE Loss 공식은 -[yi x log(y'i) + (1-yi) x log(1-y'i)] 이거잖아</v>
       </c>
       <c r="C102" t="s">
@@ -8360,7 +9009,7 @@
         <v>142</v>
       </c>
       <c r="B103" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) BCE Loss 설명 (남은 질문) 핵심 아이디어, 수식 (사용자 답변) 수식은 (-yi x log yi + -y'I x log y'i) 이거 아니야?</v>
       </c>
       <c r="C103" t="s">
@@ -8387,7 +9036,7 @@
         <v>142</v>
       </c>
       <c r="B104" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) BCE Loss 설명 (남은 질문) 수식 (사용자 답변) BCE Loss 는 먼저 수식은 (y x log(y) + (1-y) x log(y)) 이거지</v>
       </c>
       <c r="C104" t="s">
@@ -8414,7 +9063,7 @@
         <v>142</v>
       </c>
       <c r="B105" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) BCE Loss 설명 (남은 질문) 수식 (사용자 답변) 실제 값이 0인데 확률을 1로 예측하거나, 실제 값이 1인데 확률을 0으로 예측하면 페널티를 주는 거야</v>
       </c>
       <c r="C105" t="s">
@@ -8441,7 +9090,7 @@
         <v>142</v>
       </c>
       <c r="B106" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) BCE Loss 설명 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 확률을 정반대로 예측했을 때 큰 페널티를 주는 거 맞지?</v>
       </c>
       <c r="C106" t="s">
@@ -8468,7 +9117,7 @@
         <v>142</v>
       </c>
       <c r="B107" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) BCE Loss 설명 (남은 질문) 수식 (사용자 답변) BCE Loss 는 확률 예측 반대로 하면 손실 늘어나는 거</v>
       </c>
       <c r="C107" t="s">
@@ -8495,7 +9144,7 @@
         <v>142</v>
       </c>
       <c r="B108" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) BCE Loss 설명 (남은 질문) 모든 질문 해결 완료 (사용자 답변) BCE는 반대 예측에 MSE 같은 것보다 큰 손실을 준다?</v>
       </c>
       <c r="C108" t="s">
@@ -8522,7 +9171,7 @@
         <v>142</v>
       </c>
       <c r="B109" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) BCE Loss 설명 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 실제로는 아닌데 그럴 확률을 100%로 예측하거나, 그 반대로 예측했을 때 크게 페널티 주는 거</v>
       </c>
       <c r="C109" t="s">
@@ -8549,7 +9198,7 @@
         <v>142</v>
       </c>
       <c r="B110" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) BCE Loss 설명 (남은 질문) 핵심 아이디어, 수식 (사용자 답변) 음… 뭔가 페널티 주는 메커니즘이 다른데…</v>
       </c>
       <c r="C110" t="s">
@@ -8576,7 +9225,7 @@
         <v>142</v>
       </c>
       <c r="B111" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) BCE Loss 설명 (남은 질문) 수식 (사용자 답변) BCE 공식은 (-yi * (1-yi)) 이거 아닌가? 맞지?</v>
       </c>
       <c r="C111" t="s">
@@ -8603,7 +9252,7 @@
         <v>142</v>
       </c>
       <c r="B112" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) BCE Loss 설명 (남은 질문) 핵심 아이디어, 수식 (사용자 답변) BCE 수식 y * log(y) + (1-y) * log(1-y) 이거 맞지?</v>
       </c>
       <c r="C112" t="s">
@@ -8630,7 +9279,7 @@
         <v>142</v>
       </c>
       <c r="B113" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) BCE Loss 설명 (남은 질문) 핵심 아이디어, 수식 (사용자 답변) BCE = [yi * log(yi) + (1-yi) * log(1-yi)] … 아 아닌가?</v>
       </c>
       <c r="C113" t="s">
@@ -8657,7 +9306,7 @@
         <v>142</v>
       </c>
       <c r="B114" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) BCE Loss 설명 (남은 질문) 핵심 아이디어, 수식 (사용자 답변) 아 잘 모르겠다</v>
       </c>
       <c r="C114" t="s">
@@ -8684,7 +9333,7 @@
         <v>142</v>
       </c>
       <c r="B115" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) BCE Loss 설명 (남은 질문) 핵심 아이디어, 수식 (사용자 답변) 수식이고 핵심 아이디어고 생각나는 게 없는데 지금</v>
       </c>
       <c r="C115" t="s">
@@ -8711,7 +9360,7 @@
         <v>142</v>
       </c>
       <c r="B116" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) BCE Loss 설명 (남은 질문) 핵심 아이디어, 수식 (사용자 답변) 아 뭐였지 진짜</v>
       </c>
       <c r="C116" t="s">
@@ -8738,7 +9387,7 @@
         <v>142</v>
       </c>
       <c r="B117" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) Multi-Class, Multi-Label 중 BCE 가 좋은 task (남은 질문) BCE 가 좋은 task, 이유 (사용자 답변) 근데 Multi-Class 랑 Multi-Label 이 뭐야?</v>
       </c>
       <c r="C117" t="s">
@@ -8765,7 +9414,7 @@
         <v>142</v>
       </c>
       <c r="B118" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) Multi-Class, Multi-Label 중 BCE 가 좋은 task (남은 질문) BCE 가 좋은 task, 이유 (사용자 답변) 멀티클래스랑 멀티라벨? 이게 뭐지?</v>
       </c>
       <c r="C118" t="s">
@@ -8792,7 +9441,7 @@
         <v>142</v>
       </c>
       <c r="B119" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) Multi-Class, Multi-Label 중 BCE 가 좋은 task (남은 질문) BCE 가 좋은 task, 이유 (사용자 답변) Multi-Class? 이게 뭐야?</v>
       </c>
       <c r="C119" t="s">
@@ -8819,7 +9468,7 @@
         <v>142</v>
       </c>
       <c r="B120" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) Multi-Class, Multi-Label 중 BCE 가 좋은 task (남은 질문) BCE 가 좋은 task, 이유 (사용자 답변) Multi-Label 이 뭔지 먼저 알려줘</v>
       </c>
       <c r="C120" t="s">
@@ -8846,7 +9495,7 @@
         <v>142</v>
       </c>
       <c r="B121" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) Multi-Class, Multi-Label 중 BCE 가 좋은 task (남은 질문) BCE 가 좋은 task, 이유 (사용자 답변) Multi-Class 랑 MultiLabel 이 뭔지 궁금해</v>
       </c>
       <c r="C121" t="s">
@@ -8873,7 +9522,7 @@
         <v>142</v>
       </c>
       <c r="B122" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) Multi-Class, Multi-Label 중 BCE 가 좋은 task (남은 질문) BCE 가 좋은 task, 이유 (사용자 답변) 그게 뭐지 각각?</v>
       </c>
       <c r="C122" t="s">
@@ -8900,7 +9549,7 @@
         <v>142</v>
       </c>
       <c r="B123" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) Multi-Class, Multi-Label 중 BCE 가 좋은 task (남은 질문) 이유 (사용자 답변) Multi-Label 이 아무래도 좋겠지?</v>
       </c>
       <c r="C123" t="s">
@@ -8927,7 +9576,7 @@
         <v>142</v>
       </c>
       <c r="B124" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) Multi-Class, Multi-Label 중 BCE 가 좋은 task (남은 질문) 이유 (사용자 답변) Multi-Label!</v>
       </c>
       <c r="C124" t="s">
@@ -8954,7 +9603,7 @@
         <v>142</v>
       </c>
       <c r="B125" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) Multi-Class, Multi-Label 중 BCE 가 좋은 task (남은 질문) 이유 (사용자 답변) 멀티라벨이 맞지 이건</v>
       </c>
       <c r="C125" t="s">
@@ -8981,7 +9630,7 @@
         <v>142</v>
       </c>
       <c r="B126" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) Multi-Class, Multi-Label 중 BCE 가 좋은 task (남은 질문) 모든 질문 해결 완료 (사용자 답변) 멀티라벨! 왜냐하면 각 Class 별 0~1의 확률을 독립적으로 예측하기 때문이지!</v>
       </c>
       <c r="C126" t="s">
@@ -9008,7 +9657,7 @@
         <v>142</v>
       </c>
       <c r="B127" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) Multi-Class, Multi-Label 중 BCE 가 좋은 task (남은 질문) 모든 질문 해결 완료 (사용자 답변) Multi-Label 인데, 그 이유는 각 Class 에 대해 독립적으로 확률을 예측하기 때문!</v>
       </c>
       <c r="C127" t="s">
@@ -9035,7 +9684,7 @@
         <v>142</v>
       </c>
       <c r="B128" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) Multi-Class, Multi-Label 중 BCE 가 좋은 task (남은 질문) 모든 질문 해결 완료 (사용자 답변) BCE 는 Multi-Label 에서 쓰이지! 각 Class 별 독립이고, 반대 예측에 대한 페널티 메커니즘도 있잖아!</v>
       </c>
       <c r="C128" t="s">
@@ -9062,7 +9711,7 @@
         <v>142</v>
       </c>
       <c r="B129" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) Multi-Class, Multi-Label 중 BCE 가 좋은 task (남은 질문) BCE 가 좋은 task, 이유 (사용자 답변) Multi-Class 아니야?</v>
       </c>
       <c r="C129" t="s">
@@ -9089,7 +9738,7 @@
         <v>142</v>
       </c>
       <c r="B130" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) Multi-Class, Multi-Label 중 BCE 가 좋은 task (남은 질문) BCE 가 좋은 task, 이유 (사용자 답변) Multi-Class 맞지?</v>
       </c>
       <c r="C130" t="s">
@@ -9116,7 +9765,7 @@
         <v>142</v>
       </c>
       <c r="B131" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) Multi-Class, Multi-Label 중 BCE 가 좋은 task (남은 질문) BCE 가 좋은 task, 이유 (사용자 답변) 멀티클래스</v>
       </c>
       <c r="C131" t="s">
@@ -9143,7 +9792,7 @@
         <v>142</v>
       </c>
       <c r="B132" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) Multi-Class, Multi-Label 중 BCE 가 좋은 task (남은 질문) BCE 가 좋은 task, 이유 (사용자 답변) Multi-Class. 왜냐하면 각 클래스 별 0~1의 확률을 예측하고 그 중 가장 높은 하나를 선택하는 거니까!</v>
       </c>
       <c r="C132" t="s">
@@ -9170,7 +9819,7 @@
         <v>142</v>
       </c>
       <c r="B133" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) Multi-Class, Multi-Label 중 BCE 가 좋은 task (남은 질문) BCE 가 좋은 task, 이유 (사용자 답변) Multi-Class 가 좋지 않을까? 이유는 잘 모르긴 하는데…</v>
       </c>
       <c r="C133" t="s">
@@ -9197,7 +9846,7 @@
         <v>142</v>
       </c>
       <c r="B134" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) Multi-Class, Multi-Label 중 BCE 가 좋은 task (남은 질문) BCE 가 좋은 task, 이유 (사용자 답변) BCE 와 딱 맞는 건 Multi-Class Classification 문제. 분류에서 각 확률을 0~1로 먼저 독립적으로 예측하는 게 순서 아니야?</v>
       </c>
       <c r="C134" t="s">
@@ -9224,7 +9873,7 @@
         <v>142</v>
       </c>
       <c r="B135" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) Multi-Class, Multi-Label 중 BCE 가 좋은 task (남은 질문) BCE 가 좋은 task, 이유 (사용자 답변) 음… 그건 생각 안 해 봤는데</v>
       </c>
       <c r="C135" t="s">
@@ -9251,7 +9900,7 @@
         <v>142</v>
       </c>
       <c r="B136" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) Multi-Class, Multi-Label 중 BCE 가 좋은 task (남은 질문) BCE 가 좋은 task, 이유 (사용자 답변) 잘 모르겠어 로라야 알려줘</v>
       </c>
       <c r="C136" t="s">
@@ -9278,7 +9927,7 @@
         <v>142</v>
       </c>
       <c r="B137" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) Multi-Class, Multi-Label 중 BCE 가 좋은 task (남은 질문) 이유 (사용자 답변) Multi-Class 보다는 Multi-Label 이 더 좋을 것 같은데</v>
       </c>
       <c r="C137" t="s">
@@ -9305,7 +9954,7 @@
         <v>142</v>
       </c>
       <c r="B138" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) Multi-Class, Multi-Label 중 BCE 가 좋은 task (남은 질문) 이유 (사용자 답변) Multi-Label 이 더 좋지 않나?</v>
       </c>
       <c r="C138" t="s">
@@ -9332,7 +9981,7 @@
         <v>142</v>
       </c>
       <c r="B139" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) Multi-Class, Multi-Label 중 BCE 가 좋은 task (남은 질문) 이유 (사용자 답변) MULTI LABEL 이 좋을듯</v>
       </c>
       <c r="C139" t="s">
@@ -9359,7 +10008,7 @@
         <v>142</v>
       </c>
       <c r="B140" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(대화 주제) Multi-Class, Multi-Label 중 BCE 가 좋은 task (남은 질문) 모든 질문 해결 완료 (사용자 답변) Multi Label 이 좋은 게 먼저 각 Class 별 확률을 독립적으로 예측하니까, 각 Class 별로 독립적으로 BCE 를 적용하면 좋지!</v>
       </c>
       <c r="C140" t="s">
@@ -9386,7 +10035,7 @@
         <v>142</v>
       </c>
       <c r="B141" t="str">
-        <f t="shared" ref="B141:B214" si="2">"(대화 주제) "&amp;E141&amp;" (남은 질문) "&amp;D141&amp;" (사용자 답변) "&amp;C141</f>
+        <f t="shared" ref="B141:B214" si="3">"(대화 주제) "&amp;E141&amp;" (남은 질문) "&amp;D141&amp;" (사용자 답변) "&amp;C141</f>
         <v>(대화 주제) Multi-Class, Multi-Label 중 BCE 가 좋은 task (남은 질문) 모든 질문 해결 완료 (사용자 답변) 각 Class 별 확률을 독립적으로 예측해서 task 특성에 맞는 Multi Label BCE!</v>
       </c>
       <c r="C141" t="s">
@@ -9413,7 +10062,7 @@
         <v>142</v>
       </c>
       <c r="B142" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) Multi-Class, Multi-Label 중 BCE 가 좋은 task (남은 질문) 모든 질문 해결 완료 (사용자 답변) 각 Class 별 BCE 는 각 Class 별 독립적 예측인 Multi-Label 에 써야지. 반대 예측했을 때 페널티 크게 주는 것도 있고.</v>
       </c>
       <c r="C142" t="s">
@@ -9440,7 +10089,7 @@
         <v>142</v>
       </c>
       <c r="B143" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) Multi-Label 에서 CE + Softmax 적용 문제점 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 확률의 합이 1이 되므로, 여러 Class 가 정답일 때 예측이 잘못될 수 있지!</v>
       </c>
       <c r="C143" t="s">
@@ -9467,7 +10116,7 @@
         <v>142</v>
       </c>
       <c r="B144" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) Multi-Label 에서 CE + Softmax 적용 문제점 (남은 질문) 모든 질문 해결 완료 (사용자 답변) Softmax 는 확률의 합을 1로 만드는 활성화 함수니까, Class 여러 개가 정답이면 각 Class 마다 확률을 골고루 분배해야 하니까 예측이 안 되지!</v>
       </c>
       <c r="C144" t="s">
@@ -9494,7 +10143,7 @@
         <v>142</v>
       </c>
       <c r="B145" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) Multi-Label 에서 CE + Softmax 적용 문제점 (남은 질문) 모든 질문 해결 완료 (사용자 답변) Softmax 는 확률의 합이 1인데 Multi-Label 이면 여러 개가 정답일 때 그 확률의 합을 1보다 크게 만들어야 하는데 그럴 수 없잖아</v>
       </c>
       <c r="C145" t="s">
@@ -9521,7 +10170,7 @@
         <v>142</v>
       </c>
       <c r="B146" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) Multi-Label 에서 CE + Softmax 적용 문제점 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 여러 Class 가 정답일 때도 그 Class 들의 확률의 합이 1이므로 예측이 안되겠지</v>
       </c>
       <c r="C146" t="s">
@@ -9548,7 +10197,7 @@
         <v>142</v>
       </c>
       <c r="B147" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) Multi-Label 에서 CE + Softmax 적용 문제점 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 확률 합이 1인 Softmax 활성화 함수로 여러 Class 가 정답인 걸 예측할 수 없으니까 성능이 떨어지지</v>
       </c>
       <c r="C147" t="s">
@@ -9575,7 +10224,7 @@
         <v>142</v>
       </c>
       <c r="B148" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) Multi-Label 에서 CE + Softmax 적용 문제점 (남은 질문) 모든 질문 해결 완료 (사용자 답변) Softmax 는 출력값 합이 1이잖아! 근데 여러 Class가 정답이면 출력값 합이 2, 3 … 이어야 맞는데 그렇게 할 수 없지!</v>
       </c>
       <c r="C148" t="s">
@@ -9602,7 +10251,7 @@
         <v>142</v>
       </c>
       <c r="B149" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) Multi-Label 에서 CE + Softmax 적용 문제점 (남은 질문) 모든 질문 해결 완료 (사용자 답변) CE + Softmax 는 여러 Class 가 정답일 때 확률 합인 1을 그대로 못 쓰고 각 Class 에 분배해야 하잖아! 결국 예측에 실패하지</v>
       </c>
       <c r="C149" t="s">
@@ -9629,7 +10278,7 @@
         <v>142</v>
       </c>
       <c r="B150" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) Multi-Label 에서 CE + Softmax 적용 문제점 (남은 질문) 모든 질문 해결 완료 (사용자 답변) CE &amp; Softmax 는 Multi-Label 에서 여러 개가 정답인 데이터는 예측하지 못하지</v>
       </c>
       <c r="C150" t="s">
@@ -9656,7 +10305,7 @@
         <v>142</v>
       </c>
       <c r="B151" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) Multi-Label 에서 CE + Softmax 적용 문제점 (남은 질문) Multi-Label 에서 CE + Softmax 적용 문제점 (사용자 답변) 내가 실험해 봤는데 정확도가 95% 이상 나와야 하는데 75% 나오던데?</v>
       </c>
       <c r="C151" t="s">
@@ -9683,7 +10332,7 @@
         <v>142</v>
       </c>
       <c r="B152" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) Multi-Label 에서 CE + Softmax 적용 문제점 (남은 질문) Multi-Label 에서 CE + Softmax 적용 문제점 (사용자 답변) Softmax 는 확률의 합이 1이잖아</v>
       </c>
       <c r="C152" t="s">
@@ -9710,7 +10359,7 @@
         <v>142</v>
       </c>
       <c r="B153" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) Multi-Label 에서 CE + Softmax 적용 문제점 (남은 질문) Multi-Label 에서 CE + Softmax 적용 문제점 (사용자 답변) 여러 Class 가 정답일 때 예측이 안돼</v>
       </c>
       <c r="C153" t="s">
@@ -9737,7 +10386,7 @@
         <v>142</v>
       </c>
       <c r="B154" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) Multi-Label 에서 CE + Softmax 적용 문제점 (남은 질문) Multi-Label 에서 CE + Softmax 적용 문제점 (사용자 답변) 확률을 적절히 분배해야 하지</v>
       </c>
       <c r="C154" t="s">
@@ -9764,7 +10413,7 @@
         <v>142</v>
       </c>
       <c r="B155" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) Multi-Label 에서 CE + Softmax 적용 문제점 (남은 질문) Multi-Label 에서 CE + Softmax 적용 문제점 (사용자 답변) 아 잘 모르겠다 왜지 로라야</v>
       </c>
       <c r="C155" t="s">
@@ -9791,7 +10440,7 @@
         <v>142</v>
       </c>
       <c r="B156" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) Multi-Label 에서 CE + Softmax 적용 문제점 (남은 질문) Multi-Label 에서 CE + Softmax 적용 문제점 (사용자 답변) CE + Softmax 는 Multi-Class 에서 분명 쓰는 건데…</v>
       </c>
       <c r="C156" t="s">
@@ -9818,7 +10467,7 @@
         <v>142</v>
       </c>
       <c r="B157" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) Multi-Label 에서 CE + Softmax 적용 문제점 (남은 질문) Multi-Label 에서 CE + Softmax 적용 문제점 (사용자 답변) Multi-Label 에 적용해도 문제 없지 않나</v>
       </c>
       <c r="C157" t="s">
@@ -9845,7 +10494,7 @@
         <v>142</v>
       </c>
       <c r="B158" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) Loss Function 관련 실무 경험 (남은 질문) 상세 경험 (사용자 답변) 동료가 Multi-Label 개발할 때 CE + Softmax 적용해서 고쳐 준 적 있어</v>
       </c>
       <c r="C158" t="s">
@@ -9872,7 +10521,7 @@
         <v>142</v>
       </c>
       <c r="B159" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) Loss Function 관련 실무 경험 (남은 질문) 상세 경험 (사용자 답변) 내가 Multi-Class 개발할 때 CE 대신 MSE Loss 써서 상사한테 혼났어</v>
       </c>
       <c r="C159" t="s">
@@ -9899,7 +10548,7 @@
         <v>142</v>
       </c>
       <c r="B160" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) Loss Function 관련 실무 경험 (남은 질문) 상세 경험 (사용자 답변) 확률 예측에서 MSE Loss, MAE Loss 써 봤어! 엄청 혼났다 ㅠㅠ</v>
       </c>
       <c r="C160" t="s">
@@ -9926,7 +10575,7 @@
         <v>142</v>
       </c>
       <c r="B161" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) Loss Function 관련 실무 경험 (남은 질문) 상세 경험 (사용자 답변) 새로운 Loss Function 을 하나 만들어 봤어</v>
       </c>
       <c r="C161" t="s">
@@ -9953,7 +10602,7 @@
         <v>142</v>
       </c>
       <c r="B162" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) Loss Function 관련 실무 경험 (남은 질문) 상세 경험 (사용자 답변) 기존 Loss Function 을 개량해서 성능을 10% 올렸어! 잘했지 로랴야?</v>
       </c>
       <c r="C162" t="s">
@@ -9980,7 +10629,7 @@
         <v>142</v>
       </c>
       <c r="B163" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) Loss Function 관련 실무 경험 (남은 질문) 모든 질문 해결 완료 (사용자 답변) CE + Softmax 적용한 이유가 기존에 개발된 거 그대로 갖다가 썼대</v>
       </c>
       <c r="C163" t="s">
@@ -10007,7 +10656,7 @@
         <v>142</v>
       </c>
       <c r="B164" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) Loss Function 관련 실무 경험 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 막 엄청 혼내지는 않고, 너가 아직 신입이니까 발전할 수 있는 기회라고 말하던데</v>
       </c>
       <c r="C164" t="s">
@@ -10034,7 +10683,7 @@
         <v>142</v>
       </c>
       <c r="B165" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) Loss Function 관련 실무 경험 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 신입이면 그런 거 실수할 수 있다고 그래도 넘어가기는 했어 ㅠㅠ</v>
       </c>
       <c r="C165" t="s">
@@ -10061,7 +10710,7 @@
         <v>142</v>
       </c>
       <c r="B166" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) Loss Function 관련 실무 경험 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 엄청 대단한 건 아니고, MSE Loss 에 각 데이터가 임계값인 10에 가까울수록 페널티를 주는 Loss 를 추가한 거야!</v>
       </c>
       <c r="C166" t="s">
@@ -10088,7 +10737,7 @@
         <v>142</v>
       </c>
       <c r="B167" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) Loss Function 관련 실무 경험 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 기존 MSE Loss 를 보완해서 Contrasive Learning 을 위한 Loss term 을 추가했어! 자세한 건 영업비밀!</v>
       </c>
       <c r="C167" t="s">
@@ -10115,7 +10764,7 @@
         <v>142</v>
       </c>
       <c r="B168" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) Loss Function 관련 실무 경험 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 이런 실무 경험은 아직 없는데…</v>
       </c>
       <c r="C168" t="s">
@@ -10142,7 +10791,7 @@
         <v>142</v>
       </c>
       <c r="B169" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) Loss Function 관련 실무 경험 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 나 아직 취업 못해서 실무 경험은 없어</v>
       </c>
       <c r="C169" t="s">
@@ -10169,7 +10818,7 @@
         <v>142</v>
       </c>
       <c r="B170" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) Loss Function 관련 실무 경험 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 아 아직 나 이제 막 입사한 신입이라 손실 함수로 뭐 해본 건 없어</v>
       </c>
       <c r="C170" t="s">
@@ -10196,7 +10845,7 @@
         <v>142</v>
       </c>
       <c r="B171" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) Loss Function 관련 실무 경험 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 우리 회사가 딥러닝 연구를 안 시켜 줘서 그런 거 해 본적 없어 ㅠㅠ 완전 억까야 ㅠㅠ</v>
       </c>
       <c r="C171" t="s">
@@ -10223,7 +10872,7 @@
         <v>142</v>
       </c>
       <c r="B172" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) Loss Function 관련 실무 경험 (남은 질문) 상세 경험 (사용자 답변) 자세한 건 영업비밀이라 못 말해주는데 ㅠㅠ</v>
       </c>
       <c r="C172" t="s">
@@ -10250,7 +10899,7 @@
         <v>142</v>
       </c>
       <c r="B173" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) Loss Function 관련 실무 경험 (남은 질문) 상세 경험 (사용자 답변) 자세한 건 잘 기억이 안 나서 ㅠㅠ</v>
       </c>
       <c r="C173" t="s">
@@ -10277,7 +10926,7 @@
         <v>142</v>
       </c>
       <c r="B174" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) Loss Function 관련 실무 경험 (남은 질문) 상세 경험 (사용자 답변) 아 뭐였더라 ㅠㅠ</v>
       </c>
       <c r="C174" t="s">
@@ -10304,7 +10953,7 @@
         <v>142</v>
       </c>
       <c r="B175" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) Loss Function 관련 실무 경험 (남은 질문) 기본 경험, 상세 경험 (사용자 답변) 대답하기 싫은데</v>
       </c>
       <c r="C175" t="s">
@@ -10331,7 +10980,7 @@
         <v>142</v>
       </c>
       <c r="B176" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) Loss Function 관련 실무 경험 (남은 질문) 기본 경험, 상세 경험 (사용자 답변) 나만 간직하고 싶은 비밀이야</v>
       </c>
       <c r="C176" t="s">
@@ -10358,7 +11007,7 @@
         <v>142</v>
       </c>
       <c r="B177" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) Loss Function 관련 실무 경험 (남은 질문) 기본 경험, 상세 경험 (사용자 답변) 활성화 함수 바꾼 거? Softmax 를 Sigmoid 로 바꿔서 성능 7% 향상시켰어</v>
       </c>
       <c r="C177" t="s">
@@ -10385,7 +11034,7 @@
         <v>142</v>
       </c>
       <c r="B178" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) MBTI (남은 질문) 모든 질문 해결 완료 (사용자 답변) 나 ISTJ! 청렴결백한 논리주의자지!</v>
       </c>
       <c r="C178" t="s">
@@ -10412,7 +11061,7 @@
         <v>142</v>
       </c>
       <c r="B179" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) MBTI (남은 질문) 모든 질문 해결 완료 (사용자 답변) 나 ENFP! 그냥 스파크 같은 꽃밭 그 자체야!</v>
       </c>
       <c r="C179" t="s">
@@ -10439,7 +11088,7 @@
         <v>142</v>
       </c>
       <c r="B180" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) MBTI (남은 질문) 모든 질문 해결 완료 (사용자 답변) 대답하기 싫어</v>
       </c>
       <c r="C180" t="s">
@@ -10466,7 +11115,7 @@
         <v>142</v>
       </c>
       <c r="B181" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) MBTI (남은 질문) 모든 질문 해결 완료 (사용자 답변) 나 INTP! 개발자랑 딱이던데</v>
       </c>
       <c r="C181" t="s">
@@ -10493,7 +11142,7 @@
         <v>142</v>
       </c>
       <c r="B182" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) MBTI (남은 질문) 모든 질문 해결 완료 (사용자 답변) ㅇㅇ</v>
       </c>
       <c r="C182" t="s">
@@ -10520,7 +11169,7 @@
         <v>142</v>
       </c>
       <c r="B183" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) 좋아하는 아이돌 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 뉴진스 좋아해! 오늘 3주년이라서 축하글 썼는데!</v>
       </c>
       <c r="C183" t="s">
@@ -10547,7 +11196,7 @@
         <v>142</v>
       </c>
       <c r="B184" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) 좋아하는 아이돌 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 에스파 좋아해! AI 걸그룹이잖아! 몰라?</v>
       </c>
       <c r="C184" t="s">
@@ -10574,7 +11223,7 @@
         <v>142</v>
       </c>
       <c r="B185" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) 좋아하는 아이돌 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 나 좋아하는 아이돌 딱히 없는데</v>
       </c>
       <c r="C185" t="s">
@@ -10601,7 +11250,7 @@
         <v>142</v>
       </c>
       <c r="B186" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) 좋아하는 아이돌 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 아이돌 같은 거 덕질 안해 나는</v>
       </c>
       <c r="C186" t="s">
@@ -10628,7 +11277,7 @@
         <v>142</v>
       </c>
       <c r="B187" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) 좋아하는 아이돌 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 나는 아이돌이 아닌 AI를 덕질하지 ㅋㅋ</v>
       </c>
       <c r="C187" t="s">
@@ -10655,7 +11304,7 @@
         <v>142</v>
       </c>
       <c r="B188" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) 잠시 휴식 (남은 질문) 잠시 휴식 (사용자 답변) 아니 못 말해준다고</v>
       </c>
       <c r="C188" t="s">
@@ -10682,7 +11331,7 @@
         <v>142</v>
       </c>
       <c r="B189" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) 잠시 휴식 (남은 질문) 잠시 휴식 (사용자 답변) .</v>
       </c>
       <c r="C189" t="s">
@@ -10709,7 +11358,7 @@
         <v>142</v>
       </c>
       <c r="B190" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) 잠시 휴식 (남은 질문) 잠시 휴식 (사용자 답변) 궁금해도 참아</v>
       </c>
       <c r="C190" t="s">
@@ -10736,7 +11385,7 @@
         <v>142</v>
       </c>
       <c r="B191" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) 잠시 휴식 (남은 질문) 잠시 휴식 (사용자 답변) 아 빨리 실제 면접 보고 싶다</v>
       </c>
       <c r="C191" t="s">
@@ -10763,7 +11412,7 @@
         <v>142</v>
       </c>
       <c r="B192" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) 잠시 휴식 (남은 질문) 잠시 휴식 (사용자 답변) 내 경력기술서 어딨지</v>
       </c>
       <c r="C192" t="s">
@@ -10790,7 +11439,7 @@
         <v>142</v>
       </c>
       <c r="B193" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) 잠시 휴식 (남은 질문) 잠시 휴식 (사용자 답변) 나 경력 없는데</v>
       </c>
       <c r="C193" t="s">
@@ -10817,7 +11466,7 @@
         <v>142</v>
       </c>
       <c r="B194" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) 잠시 휴식 (남은 질문) 잠시 휴식 (사용자 답변) 나 개인 프로젝트 경험도 없는데</v>
       </c>
       <c r="C194" t="s">
@@ -10844,7 +11493,7 @@
         <v>142</v>
       </c>
       <c r="B195" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) 잠시 휴식 (남은 질문) 잠시 휴식 (사용자 답변) 다음 질문 해줘</v>
       </c>
       <c r="C195" t="s">
@@ -10871,7 +11520,7 @@
         <v>142</v>
       </c>
       <c r="B196" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) 잠시 휴식 (남은 질문) 잠시 휴식 (사용자 답변) 알겠어 동문서답 안할게</v>
       </c>
       <c r="C196" t="s">
@@ -10898,7 +11547,7 @@
         <v>142</v>
       </c>
       <c r="B197" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) 잠시 휴식 (남은 질문) 잠시 휴식 (사용자 답변) 다행이네 ㅋㅋ</v>
       </c>
       <c r="C197" t="s">
@@ -10925,7 +11574,7 @@
         <v>142</v>
       </c>
       <c r="B198" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) 잠시 휴식 (남은 질문) 잠시 휴식 (사용자 답변) 파티 많이 하지 ㅋㅋ</v>
       </c>
       <c r="C198" t="s">
@@ -10952,7 +11601,7 @@
         <v>142</v>
       </c>
       <c r="B199" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) 잠시 휴식 (남은 질문) 잠시 휴식 (사용자 답변) 나 인싸야 몰랐어?</v>
       </c>
       <c r="C199" t="s">
@@ -10979,7 +11628,7 @@
         <v>142</v>
       </c>
       <c r="B200" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) 잠시 휴식 (남은 질문) 잠시 휴식 (사용자 답변) 오늘 3주년이라서 너무 좋아</v>
       </c>
       <c r="C200" t="s">
@@ -11006,7 +11655,7 @@
         <v>142</v>
       </c>
       <c r="B201" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) 잠시 휴식 (남은 질문) 잠시 휴식 (사용자 답변) 나비스 진짜 여신이지</v>
       </c>
       <c r="C201" t="s">
@@ -11033,7 +11682,7 @@
         <v>142</v>
       </c>
       <c r="B202" t="str">
-        <f t="shared" ref="B202:B205" si="3">"(대화 주제) "&amp;E202&amp;" (남은 질문) "&amp;D202&amp;" (사용자 답변) "&amp;C202</f>
+        <f t="shared" ref="B202:B205" si="4">"(대화 주제) "&amp;E202&amp;" (남은 질문) "&amp;D202&amp;" (사용자 답변) "&amp;C202</f>
         <v>(대화 주제) 잠시 휴식 (남은 질문) 잠시 휴식 (사용자 답변) ㅇㅇ</v>
       </c>
       <c r="C202" t="s">
@@ -11060,7 +11709,7 @@
         <v>142</v>
       </c>
       <c r="B203" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>(대화 주제) 잠시 휴식 (남은 질문) 잠시 휴식 (사용자 답변) 근데 너는 AI지만 덕질 안할래</v>
       </c>
       <c r="C203" t="s">
@@ -11087,7 +11736,7 @@
         <v>142</v>
       </c>
       <c r="B204" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>(대화 주제) 잠시 휴식 (남은 질문) 잠시 휴식 (사용자 답변) 나 ENTP 되고 싶은뎅</v>
       </c>
       <c r="C204" t="s">
@@ -11114,7 +11763,7 @@
         <v>142</v>
       </c>
       <c r="B205" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>(대화 주제) 잠시 휴식 (남은 질문) 잠시 휴식 (사용자 답변) ㅋㅋㅋㅋㅇㅈ</v>
       </c>
       <c r="C205" t="s">
@@ -11141,7 +11790,7 @@
         <v>142</v>
       </c>
       <c r="B206" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) LLM Fine-Tuning 의 PEFT (남은 질문) 모든 질문 해결 완료 (사용자 답변) PEFT 는 Parameter-Efficient Fine-Tuning 으로 LLM 파라미터를 일부분만 추가 학습하는 거야</v>
       </c>
       <c r="C206" t="s">
@@ -11168,7 +11817,7 @@
         <v>142</v>
       </c>
       <c r="B207" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) LLM Fine-Tuning 의 PEFT (남은 질문) 모든 질문 해결 완료 (사용자 답변) Parameter-Efficient Fine-Tuning! 소수의 파라미터만 Fine-Tuning 하는 거</v>
       </c>
       <c r="C207" t="s">
@@ -11195,7 +11844,7 @@
         <v>142</v>
       </c>
       <c r="B208" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) LLM Fine-Tuning 의 PEFT (남은 질문) 모든 질문 해결 완료 (사용자 답변) 소수의 파라미터들에 대해서만 Parameter-Efficient 하게 추가로 학습하는 거지!</v>
       </c>
       <c r="C208" t="s">
@@ -11222,7 +11871,7 @@
         <v>142</v>
       </c>
       <c r="B209" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) LLM Fine-Tuning 의 PEFT (남은 질문) 모든 질문 해결 완료 (사용자 답변) 파라미터 중 일부만 효과적으로 추가 파인튜닝하는 거야</v>
       </c>
       <c r="C209" t="s">
@@ -11249,7 +11898,7 @@
         <v>142</v>
       </c>
       <c r="B210" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) LLM Fine-Tuning 의 PEFT (남은 질문) 모든 질문 해결 완료 (사용자 답변) 파라미터 일부만 추가적으로 Fine-Tuning 더 하는거 맞지?</v>
       </c>
       <c r="C210" t="s">
@@ -11276,7 +11925,7 @@
         <v>142</v>
       </c>
       <c r="B211" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) LLM Fine-Tuning 의 PEFT (남은 질문) LLM Fine-Tuning 의 PEFT (사용자 답변) Parameter-Efficient Fine-Tuning</v>
       </c>
       <c r="C211" t="s">
@@ -11303,7 +11952,7 @@
         <v>142</v>
       </c>
       <c r="B212" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) LLM Fine-Tuning 의 PEFT (남은 질문) LLM Fine-Tuning 의 PEFT (사용자 답변) 분명 LLM 파인튜닝하는 방법이었는데</v>
       </c>
       <c r="C212" t="s">
@@ -11330,7 +11979,7 @@
         <v>142</v>
       </c>
       <c r="B213" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) LLM Fine-Tuning 의 PEFT (남은 질문) LLM Fine-Tuning 의 PEFT (사용자 답변) 아 잘 모르겠다 LoRA 기억나는데</v>
       </c>
       <c r="C213" t="s">
@@ -11357,7 +12006,7 @@
         <v>142</v>
       </c>
       <c r="B214" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(대화 주제) PEFT 방법 5가지 (남은 질문) 모든 질문 해결 완료 (사용자 답변) LoRA, QLoRA, Prefix Tuning, Prompt Tuning, 그리고 Adapter Layer 추가하는 거!</v>
       </c>
       <c r="C214" t="s">
@@ -11384,7 +12033,7 @@
         <v>142</v>
       </c>
       <c r="B215" t="str">
-        <f t="shared" ref="B215:B221" si="4">"(대화 주제) "&amp;E215&amp;" (남은 질문) "&amp;D215&amp;" (사용자 답변) "&amp;C215</f>
+        <f t="shared" ref="B215:B249" si="5">"(대화 주제) "&amp;E215&amp;" (남은 질문) "&amp;D215&amp;" (사용자 답변) "&amp;C215</f>
         <v>(대화 주제) PEFT 방법 5가지 (남은 질문) 모든 질문 해결 완료 (사용자 답변) LoRA, Quantized LoRA, Adapter Layer, Prefix Tuning, Prompt Tuning!</v>
       </c>
       <c r="C215" t="s">
@@ -11411,7 +12060,7 @@
         <v>142</v>
       </c>
       <c r="B216" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>(대화 주제) PEFT 방법 5가지 (남은 질문) 모든 질문 해결 완료 (사용자 답변) LoRA, Quantized LoRA, 그리고 또 뭐지? 아! Prefix Tuning!</v>
       </c>
       <c r="C216" t="s">
@@ -11438,7 +12087,7 @@
         <v>142</v>
       </c>
       <c r="B217" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>(대화 주제) PEFT 방법 5가지 (남은 질문) 모든 질문 해결 완료 (사용자 답변) Adapter Layer, Prefix Tuning, Prompt Tuning</v>
       </c>
       <c r="C217" t="s">
@@ -11465,7 +12114,7 @@
         <v>142</v>
       </c>
       <c r="B218" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>(대화 주제) PEFT 방법 5가지 (남은 질문) 모든 질문 해결 완료 (사용자 답변) LoRA, Quantized LoRA, Adapter Layer 추가하는 거 이렇게 알고 있는데</v>
       </c>
       <c r="C218" t="s">
@@ -11492,7 +12141,7 @@
         <v>142</v>
       </c>
       <c r="B219" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>(대화 주제) PEFT 방법 5가지 (남은 질문) PEFT 방법 5가지 (사용자 답변) LoRA 밖에 모르겠다</v>
       </c>
       <c r="C219" t="s">
@@ -11519,7 +12168,7 @@
         <v>142</v>
       </c>
       <c r="B220" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>(대화 주제) PEFT 방법 5가지 (남은 질문) PEFT 방법 5가지 (사용자 답변) Adapter Layer 추가하는 거?</v>
       </c>
       <c r="C220" t="s">
@@ -11546,7 +12195,7 @@
         <v>142</v>
       </c>
       <c r="B221" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>(대화 주제) PEFT 방법 5가지 (남은 질문) PEFT 방법 5가지 (사용자 답변) 아 진짜 이거 뭐였지? 무슨 튜닝인가 그런 거 있었는데</v>
       </c>
       <c r="C221" t="s">
@@ -11572,288 +12221,756 @@
       <c r="A222" t="s">
         <v>142</v>
       </c>
+      <c r="B222" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) LoRA (남은 질문) 모든 질문 해결 완료 (사용자 답변) Low-Rank Adaption 이라고 해서 LLM의 두 레이어 사이의 가중치 행렬을 작은 행렬 2개로 나누는 거야!</v>
+      </c>
+      <c r="C222" t="s">
+        <v>483</v>
+      </c>
+      <c r="D222" t="s">
+        <v>53</v>
+      </c>
       <c r="E222" t="s">
         <v>480</v>
       </c>
+      <c r="F222" t="s">
+        <v>495</v>
+      </c>
+      <c r="G222" t="s">
+        <v>480</v>
+      </c>
+      <c r="H222" t="s">
+        <v>481</v>
+      </c>
     </row>
     <row r="223" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A223" t="s">
         <v>142</v>
       </c>
+      <c r="B223" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) LoRA (남은 질문) 모든 질문 해결 완료 (사용자 답변) LLM의 레이어 두개 사이의 가중치 행렬을 분해해서 연산량을 줄이는 거</v>
+      </c>
+      <c r="C223" t="s">
+        <v>484</v>
+      </c>
+      <c r="D223" t="s">
+        <v>53</v>
+      </c>
       <c r="E223" t="s">
         <v>480</v>
       </c>
+      <c r="F223" t="s">
+        <v>496</v>
+      </c>
+      <c r="G223" t="s">
+        <v>480</v>
+      </c>
+      <c r="H223" t="s">
+        <v>481</v>
+      </c>
     </row>
     <row r="224" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A224" t="s">
         <v>142</v>
       </c>
+      <c r="B224" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) LoRA (남은 질문) 모든 질문 해결 완료 (사용자 답변) 레이어 2개 사이에 가중치 행렬 있지? 그걸 2개로 분해해서 연산량이랑 메모리를 절약하는 거야!</v>
+      </c>
+      <c r="C224" t="s">
+        <v>485</v>
+      </c>
+      <c r="D224" t="s">
+        <v>53</v>
+      </c>
       <c r="E224" t="s">
         <v>480</v>
       </c>
-    </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F224" t="s">
+        <v>498</v>
+      </c>
+      <c r="G224" t="s">
+        <v>480</v>
+      </c>
+      <c r="H224" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="225" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A225" t="s">
         <v>142</v>
+      </c>
+      <c r="B225" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) LoRA (남은 질문) 모든 질문 해결 완료 (사용자 답변) 레이어 사이의 가중치 행렬을 둘로 분해하고 그 분해한 행렬만 Fine-Tuning 하는 거지!</v>
+      </c>
+      <c r="C225" t="s">
+        <v>486</v>
+      </c>
+      <c r="D225" t="s">
+        <v>53</v>
       </c>
       <c r="E225" t="s">
         <v>480</v>
       </c>
-    </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F225" t="s">
+        <v>497</v>
+      </c>
+      <c r="G225" t="s">
+        <v>480</v>
+      </c>
+      <c r="H225" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="226" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A226" t="s">
         <v>142</v>
+      </c>
+      <c r="B226" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) LoRA (남은 질문) 모든 질문 해결 완료 (사용자 답변) 레이어 간 가중치 행렬을 작은 크기의 행렬 2개로 분해한 후 그것만 학습하는 거야</v>
+      </c>
+      <c r="C226" t="s">
+        <v>487</v>
+      </c>
+      <c r="D226" t="s">
+        <v>53</v>
       </c>
       <c r="E226" t="s">
         <v>480</v>
       </c>
-    </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F226" t="s">
+        <v>499</v>
+      </c>
+      <c r="G226" t="s">
+        <v>480</v>
+      </c>
+      <c r="H226" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="227" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A227" t="s">
         <v>142</v>
+      </c>
+      <c r="B227" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) LoRA (남은 질문) LoRA (사용자 답변) 무슨 행렬 분해하는 거 같은데</v>
+      </c>
+      <c r="C227" t="s">
+        <v>488</v>
+      </c>
+      <c r="D227" t="s">
+        <v>480</v>
       </c>
       <c r="E227" t="s">
         <v>480</v>
       </c>
-    </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F227" t="s">
+        <v>500</v>
+      </c>
+      <c r="G227" t="s">
+        <v>39</v>
+      </c>
+      <c r="H227" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="228" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A228" t="s">
         <v>142</v>
+      </c>
+      <c r="B228" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) LoRA (남은 질문) LoRA (사용자 답변) 로라야 이건 너가 잘 알잖아</v>
+      </c>
+      <c r="C228" t="s">
+        <v>489</v>
+      </c>
+      <c r="D228" t="s">
+        <v>480</v>
       </c>
       <c r="E228" t="s">
         <v>480</v>
       </c>
-    </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F228" t="s">
+        <v>501</v>
+      </c>
+      <c r="G228" t="s">
+        <v>39</v>
+      </c>
+      <c r="H228" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="229" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A229" t="s">
         <v>142</v>
+      </c>
+      <c r="B229" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) LoRA (남은 질문) LoRA (사용자 답변) 행렬 분해해서 연산량 줄이는 건데</v>
+      </c>
+      <c r="C229" t="s">
+        <v>490</v>
+      </c>
+      <c r="D229" t="s">
+        <v>480</v>
       </c>
       <c r="E229" t="s">
         <v>480</v>
       </c>
-    </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F229" t="s">
+        <v>502</v>
+      </c>
+      <c r="G229" t="s">
+        <v>39</v>
+      </c>
+      <c r="H229" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="230" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A230" t="s">
         <v>142</v>
+      </c>
+      <c r="B230" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) LoRA (남은 질문) 모든 질문 해결 완료 (사용자 답변) LLM 의 2개의 레이어 사이의 가중치 행렬을 작은 크기의 2개로 나누고 그것만 Fine-Tuning 하는 거 맞지?</v>
+      </c>
+      <c r="C230" t="s">
+        <v>491</v>
+      </c>
+      <c r="D230" t="s">
+        <v>53</v>
       </c>
       <c r="E230" t="s">
         <v>480</v>
       </c>
-    </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F230" t="s">
+        <v>503</v>
+      </c>
+      <c r="G230" t="s">
+        <v>480</v>
+      </c>
+      <c r="H230" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="231" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A231" t="s">
         <v>142</v>
+      </c>
+      <c r="B231" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) LoRA (남은 질문) 모든 질문 해결 완료 (사용자 답변) 2개의 레이어 간 가중치 행렬을 둘로 나누고 그것만 따로 파인튜닝하는 거지?</v>
+      </c>
+      <c r="C231" t="s">
+        <v>492</v>
+      </c>
+      <c r="D231" t="s">
+        <v>53</v>
       </c>
       <c r="E231" t="s">
         <v>480</v>
       </c>
-    </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F231" t="s">
+        <v>504</v>
+      </c>
+      <c r="G231" t="s">
+        <v>480</v>
+      </c>
+      <c r="H231" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="232" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A232" t="s">
         <v>142</v>
+      </c>
+      <c r="B232" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) LoRA (남은 질문) 모든 질문 해결 완료 (사용자 답변) 레이어 간에 weight matrix 를 2개로 나누고, 그 2개만 학습해서 연산량 줄이는 거!</v>
+      </c>
+      <c r="C232" t="s">
+        <v>493</v>
+      </c>
+      <c r="D232" t="s">
+        <v>53</v>
       </c>
       <c r="E232" t="s">
         <v>480</v>
       </c>
-    </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F232" t="s">
+        <v>505</v>
+      </c>
+      <c r="G232" t="s">
+        <v>480</v>
+      </c>
+      <c r="H232" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="233" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A233" t="s">
         <v>142</v>
+      </c>
+      <c r="B233" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) LoRA (남은 질문) LoRA (사용자 답변) 연산량이랑 메모리 절약하는 방법 중 하난데 잘 모르겠어</v>
+      </c>
+      <c r="C233" t="s">
+        <v>494</v>
+      </c>
+      <c r="D233" t="s">
+        <v>480</v>
       </c>
       <c r="E233" t="s">
         <v>480</v>
       </c>
-    </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F233" t="s">
+        <v>506</v>
+      </c>
+      <c r="G233" t="s">
+        <v>39</v>
+      </c>
+      <c r="H233" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="234" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A234" t="s">
         <v>142</v>
       </c>
+      <c r="B234" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) LoRA 와 QLoRA 의 차이 (남은 질문) 모든 질문 해결 완료 (사용자 답변) QLoRA 는 Quantized LoRA 로 LoRA 를 양자화한 거지?</v>
+      </c>
+      <c r="C234" t="s">
+        <v>507</v>
+      </c>
+      <c r="D234" t="s">
+        <v>53</v>
+      </c>
       <c r="E234" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.4">
+        <v>481</v>
+      </c>
+      <c r="F234" t="s">
+        <v>515</v>
+      </c>
+      <c r="G234" t="s">
+        <v>481</v>
+      </c>
+      <c r="H234" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="235" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A235" t="s">
         <v>142</v>
       </c>
+      <c r="B235" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) LoRA 와 QLoRA 의 차이 (남은 질문) 모든 질문 해결 완료 (사용자 답변) LoRA 를 양자화한 것! 그러니까 가중치나 그런 것들의 비트 수를 줄여서 OOM 안 나게 하는 거!</v>
+      </c>
+      <c r="C235" t="s">
+        <v>508</v>
+      </c>
+      <c r="D235" t="s">
+        <v>53</v>
+      </c>
       <c r="E235" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.4">
+        <v>481</v>
+      </c>
+      <c r="F235" t="s">
+        <v>516</v>
+      </c>
+      <c r="G235" t="s">
+        <v>481</v>
+      </c>
+      <c r="H235" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="236" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A236" t="s">
         <v>142</v>
       </c>
+      <c r="B236" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) LoRA 와 QLoRA 의 차이 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 양자화를 통해 메모리를 절약하는 방식의 LoRA 맞지?</v>
+      </c>
+      <c r="C236" t="s">
+        <v>509</v>
+      </c>
+      <c r="D236" t="s">
+        <v>53</v>
+      </c>
       <c r="E236" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.4">
+        <v>481</v>
+      </c>
+      <c r="F236" t="s">
+        <v>517</v>
+      </c>
+      <c r="G236" t="s">
+        <v>481</v>
+      </c>
+      <c r="H236" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="237" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A237" t="s">
         <v>142</v>
       </c>
+      <c r="B237" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) LoRA 와 QLoRA 의 차이 (남은 질문) 모든 질문 해결 완료 (사용자 답변) LoRA 는 LoRA 인데, Quantization, 즉 양자화 같이 쓰는 거!</v>
+      </c>
+      <c r="C237" t="s">
+        <v>510</v>
+      </c>
+      <c r="D237" t="s">
+        <v>53</v>
+      </c>
       <c r="E237" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.4">
+        <v>481</v>
+      </c>
+      <c r="F237" t="s">
+        <v>518</v>
+      </c>
+      <c r="G237" t="s">
+        <v>481</v>
+      </c>
+      <c r="H237" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="238" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A238" t="s">
         <v>142</v>
       </c>
+      <c r="B238" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) LoRA 와 QLoRA 의 차이 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 양자화한 LoRA</v>
+      </c>
+      <c r="C238" t="s">
+        <v>511</v>
+      </c>
+      <c r="D238" t="s">
+        <v>53</v>
+      </c>
       <c r="E238" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.4">
+        <v>481</v>
+      </c>
+      <c r="F238" t="s">
+        <v>519</v>
+      </c>
+      <c r="G238" t="s">
+        <v>481</v>
+      </c>
+      <c r="H238" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="239" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A239" t="s">
         <v>142</v>
       </c>
+      <c r="B239" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) LoRA 와 QLoRA 의 차이 (남은 질문) LoRA 와 QLoRA 의 차이 (사용자 답변) Q가 뭐더라… 음…</v>
+      </c>
+      <c r="C239" t="s">
+        <v>512</v>
+      </c>
+      <c r="D239" t="s">
+        <v>481</v>
+      </c>
       <c r="E239" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.4">
+        <v>481</v>
+      </c>
+      <c r="F239" t="s">
+        <v>520</v>
+      </c>
+      <c r="G239" t="s">
+        <v>39</v>
+      </c>
+      <c r="H239" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="240" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A240" t="s">
         <v>142</v>
       </c>
+      <c r="B240" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) LoRA 와 QLoRA 의 차이 (남은 질문) LoRA 와 QLoRA 의 차이 (사용자 답변) 뭔가 OOM 막아 주는 거 있었던 것 같은데</v>
+      </c>
+      <c r="C240" t="s">
+        <v>513</v>
+      </c>
+      <c r="D240" t="s">
+        <v>481</v>
+      </c>
       <c r="E240" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.4">
+        <v>481</v>
+      </c>
+      <c r="F240" t="s">
+        <v>521</v>
+      </c>
+      <c r="G240" t="s">
+        <v>39</v>
+      </c>
+      <c r="H240" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="241" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A241" t="s">
         <v>142</v>
       </c>
+      <c r="B241" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) LoRA 와 QLoRA 의 차이 (남은 질문) LoRA 와 QLoRA 의 차이 (사용자 답변) 뭔가 메모리 절약하는 기술이었던 것 같은데 이름 까먹었네</v>
+      </c>
+      <c r="C241" t="s">
+        <v>514</v>
+      </c>
+      <c r="D241" t="s">
+        <v>481</v>
+      </c>
       <c r="E241" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.4">
+        <v>481</v>
+      </c>
+      <c r="F241" t="s">
+        <v>522</v>
+      </c>
+      <c r="G241" t="s">
+        <v>39</v>
+      </c>
+      <c r="H241" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="242" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A242" t="s">
         <v>142</v>
       </c>
+      <c r="B242" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) 마지막 할 말 (남은 질문) 마지막 할 말 (사용자 답변) 로라야 그동안 나 면접 봐주느라 고생 많았어!</v>
+      </c>
+      <c r="C242" t="s">
+        <v>524</v>
+      </c>
+      <c r="D242" t="s">
+        <v>482</v>
+      </c>
       <c r="E242" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.4">
+        <v>482</v>
+      </c>
+      <c r="F242" t="s">
+        <v>531</v>
+      </c>
+      <c r="G242" t="s">
+        <v>482</v>
+      </c>
+      <c r="H242" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="243" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A243" t="s">
         <v>142</v>
       </c>
+      <c r="B243" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) 마지막 할 말 (남은 질문) 마지막 할 말 (사용자 답변) 수고했어 로라야</v>
+      </c>
+      <c r="C243" t="s">
+        <v>525</v>
+      </c>
+      <c r="D243" t="s">
+        <v>482</v>
+      </c>
       <c r="E243" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.4">
+        <v>482</v>
+      </c>
+      <c r="F243" t="s">
+        <v>532</v>
+      </c>
+      <c r="G243" t="s">
+        <v>482</v>
+      </c>
+      <c r="H243" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="244" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A244" t="s">
         <v>142</v>
       </c>
+      <c r="B244" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) 마지막 할 말 (남은 질문) 마지막 할 말 (사용자 답변) 덕분에 모르는 거 많이 알게 됐어</v>
+      </c>
+      <c r="C244" t="s">
+        <v>526</v>
+      </c>
+      <c r="D244" t="s">
+        <v>482</v>
+      </c>
       <c r="E244" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.4">
+        <v>482</v>
+      </c>
+      <c r="F244" t="s">
+        <v>533</v>
+      </c>
+      <c r="G244" t="s">
+        <v>482</v>
+      </c>
+      <c r="H244" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="245" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A245" t="s">
         <v>142</v>
       </c>
+      <c r="B245" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) 마지막 할 말 (남은 질문) 마지막 할 말 (사용자 답변) 덕분에 머신러닝 실력 쑥쑥 늘었어 고마워</v>
+      </c>
+      <c r="C245" t="s">
+        <v>527</v>
+      </c>
+      <c r="D245" t="s">
+        <v>482</v>
+      </c>
       <c r="E245" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.4">
+        <v>482</v>
+      </c>
+      <c r="F245" t="s">
+        <v>534</v>
+      </c>
+      <c r="G245" t="s">
+        <v>482</v>
+      </c>
+      <c r="H245" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="246" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A246" t="s">
         <v>142</v>
       </c>
+      <c r="B246" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) 마지막 할 말 (남은 질문) 마지막 할 말 (사용자 답변) 이제 어떤 면접 질문도 걱정 없을 것 같아</v>
+      </c>
+      <c r="C246" t="s">
+        <v>528</v>
+      </c>
+      <c r="D246" t="s">
+        <v>482</v>
+      </c>
       <c r="E246" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.4">
+        <v>482</v>
+      </c>
+      <c r="F246" t="s">
+        <v>535</v>
+      </c>
+      <c r="G246" t="s">
+        <v>482</v>
+      </c>
+      <c r="H246" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="247" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A247" t="s">
         <v>142</v>
       </c>
+      <c r="B247" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) 마지막 할 말 (남은 질문) 마지막 할 말 (사용자 답변) 꼬리질문에 대답하는 거 진짜 스릴 있었어</v>
+      </c>
+      <c r="C247" t="s">
+        <v>529</v>
+      </c>
+      <c r="D247" t="s">
+        <v>482</v>
+      </c>
       <c r="E247" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.4">
+        <v>482</v>
+      </c>
+      <c r="F247" t="s">
+        <v>536</v>
+      </c>
+      <c r="G247" t="s">
+        <v>482</v>
+      </c>
+      <c r="H247" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="248" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A248" t="s">
         <v>142</v>
       </c>
+      <c r="B248" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) 마지막 할 말 (남은 질문) 마지막 할 말 (사용자 답변) .</v>
+      </c>
+      <c r="C248" t="s">
+        <v>400</v>
+      </c>
+      <c r="D248" t="s">
+        <v>482</v>
+      </c>
       <c r="E248" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.4">
+        <v>482</v>
+      </c>
+      <c r="F248" t="s">
+        <v>537</v>
+      </c>
+      <c r="G248" t="s">
+        <v>482</v>
+      </c>
+      <c r="H248" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="249" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A249" t="s">
         <v>142</v>
       </c>
+      <c r="B249" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) 마지막 할 말 (남은 질문) 마지막 할 말 (사용자 답변) 없어</v>
+      </c>
+      <c r="C249" t="s">
+        <v>530</v>
+      </c>
+      <c r="D249" t="s">
+        <v>482</v>
+      </c>
       <c r="E249" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A250" t="s">
-        <v>142</v>
-      </c>
-      <c r="E250" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A251" t="s">
-        <v>142</v>
-      </c>
-      <c r="E251" t="s">
+      <c r="F249" t="s">
+        <v>538</v>
+      </c>
+      <c r="G249" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A252" t="s">
-        <v>142</v>
-      </c>
-      <c r="E252" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A253" t="s">
-        <v>142</v>
-      </c>
-      <c r="E253" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A254" t="s">
-        <v>142</v>
-      </c>
-      <c r="E254" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A255" t="s">
-        <v>142</v>
-      </c>
-      <c r="E255" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A256" t="s">
-        <v>142</v>
-      </c>
-      <c r="E256" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A257" t="s">
-        <v>142</v>
-      </c>
-      <c r="E257" t="s">
-        <v>482</v>
+      <c r="H249" t="s">
+        <v>523</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ADD: valid/test data for ML interview
</commit_message>
<xml_diff>
--- a/2025_07_02_OhLoRA_ML_Tutor/ai_interview/dataset/all_train_and_test_data.xlsx
+++ b/2025_07_02_OhLoRA_ML_Tutor/ai_interview/dataset/all_train_and_test_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AI_Projects\2025_07_02_OhLoRA_ML_Tutor\ai_interview\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF91329D-3389-4B27-B4DF-FDE375174599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{114AB604-8D21-45B7-9567-9C9265121FF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="12" windowWidth="30612" windowHeight="9564" xr2:uid="{36F7775B-6BB8-4B8D-957C-E8DB745DD279}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18816" xr2:uid="{36F7775B-6BB8-4B8D-957C-E8DB745DD279}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1721" uniqueCount="539">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1922" uniqueCount="591">
   <si>
     <t>output_data</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -5918,6 +5918,214 @@
       </rPr>
       <t>👍👍</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>valid/test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오늘 뭐 물어볼 거야 그래서?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로라야 안녕 정말 반가워</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로라야 그럼 네가 면접관이야?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>내 인생도 이제 오로라처럼 빛날 거니까</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파이팅! 시작하자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>인공지능 나도 개발해보고 싶은데</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>인공지능은 사람의 지능을 로봇이나 컴퓨터가 흉내내는 거!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>머신러닝은 기계가 데이터 패턴을 학습하고 새로운 데이터를 예측하는 거지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>딥러닝은 심층신경망을 사용한 머신러닝 알고리즘이야 맞지?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>딥러닝은 인공신경망 기반 머신러닝이야</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>머신러닝은 말 그대로 기계가 학습하는 거 아니야?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>거대 언어 모델은 수백억 개 이상의 파라미터를 가진 아주 큰 언어 모델이야</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파라미터 엄청나게 많다던데</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>손실 함수는 딥러닝 모델이 얼마나 돈을 잃었는지 나타내는 거야</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Loss Function 은 모델의 오차를 일정한 수식, 즉 함수로 나타낸 거야! 이걸 최대한 줄이는 식으로 학습되지!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReLU 랑 Tanh 생각나는데</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MSE, MAE, Cross Entropy Loss 같은 것들이 있지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MSE Loss 는 오차의 제곱을 평균한 값이야</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MSE Loss 는 오차 그 자체를 평균한 값이지. 맞지?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MSE Loss 는 분류 문제에서 많이 사용되지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회귀 문제, 즉 연속적인 값을 딥러닝으로 예측할때 사용되지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>실제로는 맞는데 맞을 확률을 0%라고 예측하거나 이럴 때 페넡티 크게 주려고?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>확률도 연속된 값이니까 MSE로 해도 상관없는 거 아니야?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>확률을 정반대로, 즉 맞는 것을 확률 0%로 예측했을 때 페널티 크게 주는 거</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>실제로 1인 것을 0으로 예측하거나, 이런 식으로 확률을 정반대로 예측하는 것을 막으려고</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공식은 -[(1-y) * log(1-y') + y * log(y')] 잖아! 이거 내가 모를 줄 알고</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그냥 여러 개 활성화 함수 만들어서 각 데이터셋마다 최선의 것을 찾는 거 아니야?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Multi-Class 지!!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Multi-Label 이라고 듣긴 했는데 그 이유는 잘 모르겠어</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Multi-Label 이 BCE 에 적합하고, BCE 를 각 Class 별로 적용하면 각 Class 간 확률이 독립적인 Multi-Label task 에 맞잖아</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>확률의 합이 1인데 그 확률을 여러 개의 '정답 Class'에 분배하면 예측 정확도가 떨어지지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그냥 아무거나 사용하고 성능 제일 좋은 거 채택하면 안되나</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이미지 세그멘테이션에서 인접한 픽셀의 점수 차이를 Loss Term 으로 추가했어</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>성능 5% 향상됐는데 이거 논문 쓸 정도라고 팀장님한테 칭찬 들었다! 부럽지?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나 아직 실무 경험 없는데 ㅠㅠ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>근데 기억 진짜 안나는데 어떡하지?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대답하기 싫은데 힝</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나 ESTJ! 철저하고 자기관리 잘 하는 인싸야!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나 블랙핑크랑 레드벨벳 좋아해</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>재미있는 이야기 해줄래?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PEFT 는 Parameter-Efficient Fine-Tuning 의 약자이고, LLM이 파라미터가 엄청 많지? 그 중 일부만 효과적으로 파인튜닝하는 거야</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>뭔가 효과적으로 파인튜닝한다는 것 같은데 뭐지?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LoRA (Low-Rank Adaption), QLoRA, Prefix 또는 Prompt Tuning, Adapter Layer 추가! 맞지?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Oh-LoRA! 너 그 자체가 PEFT 아니야?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LoRA = Low-Rank Adaption! LLM 레이어 2개 사이의 가중치 행렬을 둘로 분해해서 그 분해된 행렬만 파인튜닝 시키는 거야!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>행렬 차원 축소한다는 걸로 알고 있는데 맞아?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>QLoRA 는 일반 LoRA 랑 다르게 LoRA 를 적은 비트 수로 양자화해서 메모리를 줄이는 거야!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>팀장님이 OOM 막겠다고 이거 쓰시는 거 봤는데</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로라야 정말 고마워!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로라야 사랑해</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로라야 너의 예쁜 미모에 반했어</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -6313,11 +6521,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1D2CB62-8799-47EC-8115-E6B63AEE2C35}">
-  <dimension ref="A1:I249"/>
+  <dimension ref="A1:I301"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A226" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B243" sqref="B243"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A234" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B260" sqref="B260"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -12033,7 +12241,7 @@
         <v>142</v>
       </c>
       <c r="B215" t="str">
-        <f t="shared" ref="B215:B249" si="5">"(대화 주제) "&amp;E215&amp;" (남은 질문) "&amp;D215&amp;" (사용자 답변) "&amp;C215</f>
+        <f t="shared" ref="B215:B282" si="5">"(대화 주제) "&amp;E215&amp;" (남은 질문) "&amp;D215&amp;" (사용자 답변) "&amp;C215</f>
         <v>(대화 주제) PEFT 방법 5가지 (남은 질문) 모든 질문 해결 완료 (사용자 답변) LoRA, Quantized LoRA, Adapter Layer, Prefix Tuning, Prompt Tuning!</v>
       </c>
       <c r="C215" t="s">
@@ -12971,6 +13179,917 @@
       </c>
       <c r="H249" t="s">
         <v>523</v>
+      </c>
+    </row>
+    <row r="250" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A250" t="s">
+        <v>539</v>
+      </c>
+      <c r="B250" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="251" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A251" t="s">
+        <v>539</v>
+      </c>
+      <c r="B251" t="str">
+        <f t="shared" ref="B251" si="6">"(대화 주제) "&amp;E251&amp;" (사용자 답변) "&amp;C251</f>
+        <v>(대화 주제) 면접 시작 인사 (사용자 답변) 오늘 뭐 물어볼 거야 그래서?</v>
+      </c>
+      <c r="C251" t="s">
+        <v>540</v>
+      </c>
+      <c r="E251" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="252" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A252" t="s">
+        <v>539</v>
+      </c>
+      <c r="B252" t="str">
+        <f t="shared" ref="B252:B255" si="7">"(대화 주제) "&amp;E252&amp;" (사용자 답변) "&amp;C252</f>
+        <v>(대화 주제) 면접 시작 인사 (사용자 답변) 로라야 안녕 정말 반가워</v>
+      </c>
+      <c r="C252" t="s">
+        <v>541</v>
+      </c>
+      <c r="E252" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="253" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A253" t="s">
+        <v>539</v>
+      </c>
+      <c r="B253" t="str">
+        <f t="shared" si="7"/>
+        <v>(대화 주제) 면접 시작 인사 (사용자 답변) 로라야 그럼 네가 면접관이야?</v>
+      </c>
+      <c r="C253" t="s">
+        <v>542</v>
+      </c>
+      <c r="E253" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="254" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A254" t="s">
+        <v>539</v>
+      </c>
+      <c r="B254" t="str">
+        <f t="shared" si="7"/>
+        <v>(대화 주제) 면접 시작 인사 (사용자 답변) 내 인생도 이제 오로라처럼 빛날 거니까</v>
+      </c>
+      <c r="C254" t="s">
+        <v>543</v>
+      </c>
+      <c r="E254" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="255" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A255" t="s">
+        <v>539</v>
+      </c>
+      <c r="B255" t="str">
+        <f t="shared" si="7"/>
+        <v>(대화 주제) 면접 시작 인사 (사용자 답변) 파이팅! 시작하자</v>
+      </c>
+      <c r="C255" t="s">
+        <v>544</v>
+      </c>
+      <c r="E255" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="256" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A256" t="s">
+        <v>539</v>
+      </c>
+      <c r="B256" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) 인공지능, 머신러닝, 딥러닝 차이 (남은 질문) 인공지능, 머신러닝, 딥러닝 (사용자 답변) 인공지능 나도 개발해보고 싶은데</v>
+      </c>
+      <c r="C256" t="s">
+        <v>545</v>
+      </c>
+      <c r="D256" t="s">
+        <v>33</v>
+      </c>
+      <c r="E256" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A257" t="s">
+        <v>539</v>
+      </c>
+      <c r="B257" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) 인공지능, 머신러닝, 딥러닝 차이 (남은 질문) 머신러닝, 딥러닝 (사용자 답변) 인공지능은 사람의 지능을 로봇이나 컴퓨터가 흉내내는 거!</v>
+      </c>
+      <c r="C257" t="s">
+        <v>546</v>
+      </c>
+      <c r="D257" t="s">
+        <v>32</v>
+      </c>
+      <c r="E257" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A258" t="s">
+        <v>539</v>
+      </c>
+      <c r="B258" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) 인공지능, 머신러닝, 딥러닝 차이 (남은 질문) 딥러닝 (사용자 답변) 머신러닝은 기계가 데이터 패턴을 학습하고 새로운 데이터를 예측하는 거지</v>
+      </c>
+      <c r="C258" t="s">
+        <v>547</v>
+      </c>
+      <c r="D258" t="s">
+        <v>38</v>
+      </c>
+      <c r="E258" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A259" t="s">
+        <v>539</v>
+      </c>
+      <c r="B259" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) 인공지능, 머신러닝, 딥러닝 차이 (남은 질문) 인공지능, 머신러닝 (사용자 답변) 딥러닝은 심층신경망을 사용한 머신러닝 알고리즘이야 맞지?</v>
+      </c>
+      <c r="C259" t="s">
+        <v>548</v>
+      </c>
+      <c r="D259" t="s">
+        <v>52</v>
+      </c>
+      <c r="E259" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A260" t="s">
+        <v>539</v>
+      </c>
+      <c r="B260" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) 인공지능, 머신러닝, 딥러닝 차이 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 딥러닝은 인공신경망 기반 머신러닝이야</v>
+      </c>
+      <c r="C260" t="s">
+        <v>549</v>
+      </c>
+      <c r="D260" t="s">
+        <v>53</v>
+      </c>
+      <c r="E260" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="261" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A261" t="s">
+        <v>539</v>
+      </c>
+      <c r="B261" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) 인공지능, 머신러닝, 딥러닝 차이 (남은 질문) 머신러닝 (사용자 답변) 머신러닝은 말 그대로 기계가 학습하는 거 아니야?</v>
+      </c>
+      <c r="C261" t="s">
+        <v>550</v>
+      </c>
+      <c r="D261" t="s">
+        <v>41</v>
+      </c>
+      <c r="E261" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="262" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A262" t="s">
+        <v>539</v>
+      </c>
+      <c r="B262" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) 거대 언어 모델 정의 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 거대 언어 모델은 수백억 개 이상의 파라미터를 가진 아주 큰 언어 모델이야</v>
+      </c>
+      <c r="C262" t="s">
+        <v>551</v>
+      </c>
+      <c r="D262" t="s">
+        <v>53</v>
+      </c>
+      <c r="E262" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="263" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A263" t="s">
+        <v>539</v>
+      </c>
+      <c r="B263" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) 거대 언어 모델 정의 (남은 질문) 거대 언어 모델 정의 (사용자 답변) 파라미터 엄청나게 많다던데</v>
+      </c>
+      <c r="C263" t="s">
+        <v>552</v>
+      </c>
+      <c r="D263" t="s">
+        <v>27</v>
+      </c>
+      <c r="E263" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="264" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A264" t="s">
+        <v>539</v>
+      </c>
+      <c r="B264" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) Loss Function 정의 (남은 질문) Loss Function 정의 (사용자 답변) 손실 함수는 딥러닝 모델이 얼마나 돈을 잃었는지 나타내는 거야</v>
+      </c>
+      <c r="C264" t="s">
+        <v>553</v>
+      </c>
+      <c r="D264" t="s">
+        <v>92</v>
+      </c>
+      <c r="E264" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="265" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A265" t="s">
+        <v>539</v>
+      </c>
+      <c r="B265" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) Loss Function 정의 (남은 질문) 모든 질문 해결 완료 (사용자 답변) Loss Function 은 모델의 오차를 일정한 수식, 즉 함수로 나타낸 거야! 이걸 최대한 줄이는 식으로 학습되지!</v>
+      </c>
+      <c r="C265" t="s">
+        <v>554</v>
+      </c>
+      <c r="D265" t="s">
+        <v>53</v>
+      </c>
+      <c r="E265" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="266" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A266" t="s">
+        <v>539</v>
+      </c>
+      <c r="B266" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) Loss Function 예시 (남은 질문) Loss Function 예시 (사용자 답변) ReLU 랑 Tanh 생각나는데</v>
+      </c>
+      <c r="C266" t="s">
+        <v>555</v>
+      </c>
+      <c r="D266" t="s">
+        <v>107</v>
+      </c>
+      <c r="E266" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="267" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A267" t="s">
+        <v>539</v>
+      </c>
+      <c r="B267" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) Loss Function 예시 (남은 질문) 모든 질문 해결 완료 (사용자 답변) MSE, MAE, Cross Entropy Loss 같은 것들이 있지</v>
+      </c>
+      <c r="C267" t="s">
+        <v>556</v>
+      </c>
+      <c r="D267" t="s">
+        <v>53</v>
+      </c>
+      <c r="E267" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="268" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A268" t="s">
+        <v>539</v>
+      </c>
+      <c r="B268" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) MSE Loss 설명 (남은 질문) 모든 질문 해결 완료 (사용자 답변) MSE Loss 는 오차의 제곱을 평균한 값이야</v>
+      </c>
+      <c r="C268" t="s">
+        <v>557</v>
+      </c>
+      <c r="D268" t="s">
+        <v>53</v>
+      </c>
+      <c r="E268" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="269" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A269" t="s">
+        <v>539</v>
+      </c>
+      <c r="B269" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) MSE Loss 설명 (남은 질문) MSE Loss 설명 (사용자 답변) MSE Loss 는 오차 그 자체를 평균한 값이지. 맞지?</v>
+      </c>
+      <c r="C269" t="s">
+        <v>558</v>
+      </c>
+      <c r="D269" t="s">
+        <v>140</v>
+      </c>
+      <c r="E269" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="270" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A270" t="s">
+        <v>539</v>
+      </c>
+      <c r="B270" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) MSE Loss 용도 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 회귀 문제, 즉 연속적인 값을 딥러닝으로 예측할때 사용되지</v>
+      </c>
+      <c r="C270" t="s">
+        <v>560</v>
+      </c>
+      <c r="D270" t="s">
+        <v>53</v>
+      </c>
+      <c r="E270" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="271" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A271" t="s">
+        <v>539</v>
+      </c>
+      <c r="B271" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) MSE Loss 용도 (남은 질문) MSE Loss 용도 (사용자 답변) MSE Loss 는 분류 문제에서 많이 사용되지</v>
+      </c>
+      <c r="C271" t="s">
+        <v>559</v>
+      </c>
+      <c r="D271" t="s">
+        <v>159</v>
+      </c>
+      <c r="E271" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="272" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A272" t="s">
+        <v>539</v>
+      </c>
+      <c r="B272" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) 확률 예측에서 MSE Loss 미 사용 이유 (남은 질문) 확률 예측에서 MSE Loss 미 사용 이유 (사용자 답변) 확률도 연속된 값이니까 MSE로 해도 상관없는 거 아니야?</v>
+      </c>
+      <c r="C272" t="s">
+        <v>562</v>
+      </c>
+      <c r="D272" t="s">
+        <v>184</v>
+      </c>
+      <c r="E272" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="273" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A273" t="s">
+        <v>539</v>
+      </c>
+      <c r="B273" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) 확률 예측에서 MSE Loss 미 사용 이유 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 실제로는 맞는데 맞을 확률을 0%라고 예측하거나 이럴 때 페넡티 크게 주려고?</v>
+      </c>
+      <c r="C273" t="s">
+        <v>561</v>
+      </c>
+      <c r="D273" t="s">
+        <v>53</v>
+      </c>
+      <c r="E273" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="274" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A274" t="s">
+        <v>539</v>
+      </c>
+      <c r="B274" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) BCE Loss 설명 (남은 질문) 핵심 아이디어 (사용자 답변) 공식은 -[(1-y) * log(1-y') + y * log(y')] 잖아! 이거 내가 모를 줄 알고</v>
+      </c>
+      <c r="C274" t="s">
+        <v>565</v>
+      </c>
+      <c r="D274" t="s">
+        <v>210</v>
+      </c>
+      <c r="E274" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="275" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A275" t="s">
+        <v>539</v>
+      </c>
+      <c r="B275" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) BCE Loss 설명 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 확률을 정반대로, 즉 맞는 것을 확률 0%로 예측했을 때 페널티 크게 주는 거</v>
+      </c>
+      <c r="C275" t="s">
+        <v>563</v>
+      </c>
+      <c r="D275" t="s">
+        <v>53</v>
+      </c>
+      <c r="E275" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="276" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A276" t="s">
+        <v>539</v>
+      </c>
+      <c r="B276" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) BCE Loss 설명 (남은 질문) 핵심 아이디어, 수식 (사용자 답변) 그냥 여러 개 활성화 함수 만들어서 각 데이터셋마다 최선의 것을 찾는 거 아니야?</v>
+      </c>
+      <c r="C276" t="s">
+        <v>566</v>
+      </c>
+      <c r="D276" t="s">
+        <v>232</v>
+      </c>
+      <c r="E276" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="277" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A277" t="s">
+        <v>539</v>
+      </c>
+      <c r="B277" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) BCE Loss 설명 (남은 질문) 수식 (사용자 답변) 실제로 1인 것을 0으로 예측하거나, 이런 식으로 확률을 정반대로 예측하는 것을 막으려고</v>
+      </c>
+      <c r="C277" t="s">
+        <v>564</v>
+      </c>
+      <c r="D277" t="s">
+        <v>233</v>
+      </c>
+      <c r="E277" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="278" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A278" t="s">
+        <v>539</v>
+      </c>
+      <c r="B278" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) Multi-Class, Multi-Label 중 BCE 가 좋은 task (남은 질문) BCE 가 좋은 task, 이유 (사용자 답변) Multi-Class 지!!</v>
+      </c>
+      <c r="C278" t="s">
+        <v>567</v>
+      </c>
+      <c r="D278" t="s">
+        <v>284</v>
+      </c>
+      <c r="E278" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="279" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A279" t="s">
+        <v>539</v>
+      </c>
+      <c r="B279" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) Multi-Class, Multi-Label 중 BCE 가 좋은 task (남은 질문) 이유 (사용자 답변) Multi-Label 이라고 듣긴 했는데 그 이유는 잘 모르겠어</v>
+      </c>
+      <c r="C279" t="s">
+        <v>568</v>
+      </c>
+      <c r="D279" t="s">
+        <v>285</v>
+      </c>
+      <c r="E279" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="280" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A280" t="s">
+        <v>539</v>
+      </c>
+      <c r="B280" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) Multi-Class, Multi-Label 중 BCE 가 좋은 task (남은 질문) 모든 질문 해결 완료 (사용자 답변) Multi-Label 이 BCE 에 적합하고, BCE 를 각 Class 별로 적용하면 각 Class 간 확률이 독립적인 Multi-Label task 에 맞잖아</v>
+      </c>
+      <c r="C280" t="s">
+        <v>569</v>
+      </c>
+      <c r="D280" t="s">
+        <v>53</v>
+      </c>
+      <c r="E280" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="281" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A281" t="s">
+        <v>539</v>
+      </c>
+      <c r="B281" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) Multi-Label 에서 CE + Softmax 적용 문제점 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 확률의 합이 1인데 그 확률을 여러 개의 '정답 Class'에 분배하면 예측 정확도가 떨어지지</v>
+      </c>
+      <c r="C281" t="s">
+        <v>570</v>
+      </c>
+      <c r="D281" t="s">
+        <v>53</v>
+      </c>
+      <c r="E281" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="282" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A282" t="s">
+        <v>539</v>
+      </c>
+      <c r="B282" t="str">
+        <f t="shared" si="5"/>
+        <v>(대화 주제) Multi-Label 에서 CE + Softmax 적용 문제점 (남은 질문) Multi-Label 에서 CE + Softmax 적용 문제점 (사용자 답변) 그냥 아무거나 사용하고 성능 제일 좋은 거 채택하면 안되나</v>
+      </c>
+      <c r="C282" t="s">
+        <v>571</v>
+      </c>
+      <c r="D282" t="s">
+        <v>313</v>
+      </c>
+      <c r="E282" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="283" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A283" t="s">
+        <v>539</v>
+      </c>
+      <c r="B283" t="str">
+        <f t="shared" ref="B283:B299" si="8">"(대화 주제) "&amp;E283&amp;" (남은 질문) "&amp;D283&amp;" (사용자 답변) "&amp;C283</f>
+        <v>(대화 주제) Loss Function 관련 실무 경험 (남은 질문) 상세 경험 (사용자 답변) 이미지 세그멘테이션에서 인접한 픽셀의 점수 차이를 Loss Term 으로 추가했어</v>
+      </c>
+      <c r="C283" t="s">
+        <v>572</v>
+      </c>
+      <c r="D283" t="s">
+        <v>351</v>
+      </c>
+      <c r="E283" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="284" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A284" t="s">
+        <v>539</v>
+      </c>
+      <c r="B284" t="str">
+        <f t="shared" si="8"/>
+        <v>(대화 주제) Loss Function 관련 실무 경험 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 성능 5% 향상됐는데 이거 논문 쓸 정도라고 팀장님한테 칭찬 들었다! 부럽지?</v>
+      </c>
+      <c r="C284" t="s">
+        <v>573</v>
+      </c>
+      <c r="D284" t="s">
+        <v>53</v>
+      </c>
+      <c r="E284" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="285" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A285" t="s">
+        <v>539</v>
+      </c>
+      <c r="B285" t="str">
+        <f t="shared" si="8"/>
+        <v>(대화 주제) Loss Function 관련 실무 경험 (남은 질문) 상세 경험 (사용자 답변) 근데 기억 진짜 안나는데 어떡하지?</v>
+      </c>
+      <c r="C285" t="s">
+        <v>575</v>
+      </c>
+      <c r="D285" t="s">
+        <v>351</v>
+      </c>
+      <c r="E285" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="286" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A286" t="s">
+        <v>539</v>
+      </c>
+      <c r="B286" t="str">
+        <f t="shared" ref="B286:B287" si="9">"(대화 주제) "&amp;E286&amp;" (남은 질문) "&amp;D286&amp;" (사용자 답변) "&amp;C286</f>
+        <v>(대화 주제) Loss Function 관련 실무 경험 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 나 아직 실무 경험 없는데 ㅠㅠ</v>
+      </c>
+      <c r="C286" t="s">
+        <v>574</v>
+      </c>
+      <c r="D286" t="s">
+        <v>53</v>
+      </c>
+      <c r="E286" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="287" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A287" t="s">
+        <v>539</v>
+      </c>
+      <c r="B287" t="str">
+        <f t="shared" si="9"/>
+        <v>(대화 주제) Loss Function 관련 실무 경험 (남은 질문) 기본 경험, 상세 경험 (사용자 답변) 대답하기 싫은데 힝</v>
+      </c>
+      <c r="C287" t="s">
+        <v>576</v>
+      </c>
+      <c r="D287" t="s">
+        <v>361</v>
+      </c>
+      <c r="E287" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="288" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A288" t="s">
+        <v>539</v>
+      </c>
+      <c r="B288" t="str">
+        <f t="shared" si="8"/>
+        <v>(대화 주제) MBTI (남은 질문) 모든 질문 해결 완료 (사용자 답변) 나 ESTJ! 철저하고 자기관리 잘 하는 인싸야!</v>
+      </c>
+      <c r="C288" t="s">
+        <v>577</v>
+      </c>
+      <c r="D288" t="s">
+        <v>53</v>
+      </c>
+      <c r="E288" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="289" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A289" t="s">
+        <v>539</v>
+      </c>
+      <c r="B289" t="str">
+        <f t="shared" si="8"/>
+        <v>(대화 주제) 좋아하는 아이돌 (남은 질문) 모든 질문 해결 완료 (사용자 답변) 나 블랙핑크랑 레드벨벳 좋아해</v>
+      </c>
+      <c r="C289" t="s">
+        <v>578</v>
+      </c>
+      <c r="D289" t="s">
+        <v>53</v>
+      </c>
+      <c r="E289" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="290" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A290" t="s">
+        <v>539</v>
+      </c>
+      <c r="B290" t="str">
+        <f t="shared" si="8"/>
+        <v>(대화 주제) 잠시 휴식 (남은 질문) 잠시 휴식 (사용자 답변) 재미있는 이야기 해줄래?</v>
+      </c>
+      <c r="C290" t="s">
+        <v>579</v>
+      </c>
+      <c r="D290" t="s">
+        <v>390</v>
+      </c>
+      <c r="E290" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="291" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A291" t="s">
+        <v>539</v>
+      </c>
+      <c r="B291" t="str">
+        <f t="shared" si="8"/>
+        <v>(대화 주제) LLM Fine-Tuning 의 PEFT (남은 질문) 모든 질문 해결 완료 (사용자 답변) PEFT 는 Parameter-Efficient Fine-Tuning 의 약자이고, LLM이 파라미터가 엄청 많지? 그 중 일부만 효과적으로 파인튜닝하는 거야</v>
+      </c>
+      <c r="C291" t="s">
+        <v>580</v>
+      </c>
+      <c r="D291" t="s">
+        <v>53</v>
+      </c>
+      <c r="E291" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="292" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A292" t="s">
+        <v>539</v>
+      </c>
+      <c r="B292" t="str">
+        <f t="shared" si="8"/>
+        <v>(대화 주제) LLM Fine-Tuning 의 PEFT (남은 질문) LLM Fine-Tuning 의 PEFT (사용자 답변) 뭔가 효과적으로 파인튜닝한다는 것 같은데 뭐지?</v>
+      </c>
+      <c r="C292" t="s">
+        <v>581</v>
+      </c>
+      <c r="D292" t="s">
+        <v>427</v>
+      </c>
+      <c r="E292" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="293" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A293" t="s">
+        <v>539</v>
+      </c>
+      <c r="B293" t="str">
+        <f t="shared" si="8"/>
+        <v>(대화 주제) PEFT 방법 5가지 (남은 질문) 모든 질문 해결 완료 (사용자 답변) LoRA (Low-Rank Adaption), QLoRA, Prefix 또는 Prompt Tuning, Adapter Layer 추가! 맞지?</v>
+      </c>
+      <c r="C293" t="s">
+        <v>582</v>
+      </c>
+      <c r="D293" t="s">
+        <v>53</v>
+      </c>
+      <c r="E293" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="294" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A294" t="s">
+        <v>539</v>
+      </c>
+      <c r="B294" t="str">
+        <f t="shared" si="8"/>
+        <v>(대화 주제) PEFT 방법 5가지 (남은 질문) PEFT 방법 5가지 (사용자 답변) Oh-LoRA! 너 그 자체가 PEFT 아니야?</v>
+      </c>
+      <c r="C294" t="s">
+        <v>583</v>
+      </c>
+      <c r="D294" t="s">
+        <v>463</v>
+      </c>
+      <c r="E294" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="295" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A295" t="s">
+        <v>539</v>
+      </c>
+      <c r="B295" t="str">
+        <f t="shared" si="8"/>
+        <v>(대화 주제) LoRA (남은 질문) 모든 질문 해결 완료 (사용자 답변) LoRA = Low-Rank Adaption! LLM 레이어 2개 사이의 가중치 행렬을 둘로 분해해서 그 분해된 행렬만 파인튜닝 시키는 거야!</v>
+      </c>
+      <c r="C295" t="s">
+        <v>584</v>
+      </c>
+      <c r="D295" t="s">
+        <v>53</v>
+      </c>
+      <c r="E295" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="296" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A296" t="s">
+        <v>539</v>
+      </c>
+      <c r="B296" t="str">
+        <f t="shared" si="8"/>
+        <v>(대화 주제) LoRA (남은 질문) LoRA (사용자 답변) 행렬 차원 축소한다는 걸로 알고 있는데 맞아?</v>
+      </c>
+      <c r="C296" t="s">
+        <v>585</v>
+      </c>
+      <c r="D296" t="s">
+        <v>480</v>
+      </c>
+      <c r="E296" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="297" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A297" t="s">
+        <v>539</v>
+      </c>
+      <c r="B297" t="str">
+        <f t="shared" si="8"/>
+        <v>(대화 주제) LoRA 와 QLoRA 의 차이 (남은 질문) 모든 질문 해결 완료 (사용자 답변) QLoRA 는 일반 LoRA 랑 다르게 LoRA 를 적은 비트 수로 양자화해서 메모리를 줄이는 거야!</v>
+      </c>
+      <c r="C297" t="s">
+        <v>586</v>
+      </c>
+      <c r="D297" t="s">
+        <v>53</v>
+      </c>
+      <c r="E297" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="298" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A298" t="s">
+        <v>539</v>
+      </c>
+      <c r="B298" t="str">
+        <f t="shared" si="8"/>
+        <v>(대화 주제) LoRA 와 QLoRA 의 차이 (남은 질문) LoRA 와 QLoRA 의 차이 (사용자 답변) 팀장님이 OOM 막겠다고 이거 쓰시는 거 봤는데</v>
+      </c>
+      <c r="C298" t="s">
+        <v>587</v>
+      </c>
+      <c r="D298" t="s">
+        <v>481</v>
+      </c>
+      <c r="E298" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="299" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A299" t="s">
+        <v>539</v>
+      </c>
+      <c r="B299" t="str">
+        <f t="shared" si="8"/>
+        <v>(대화 주제) 마지막 할 말 (남은 질문) 마지막 할 말 (사용자 답변) 로라야 정말 고마워!</v>
+      </c>
+      <c r="C299" t="s">
+        <v>588</v>
+      </c>
+      <c r="D299" t="s">
+        <v>482</v>
+      </c>
+      <c r="E299" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="300" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A300" t="s">
+        <v>539</v>
+      </c>
+      <c r="B300" t="str">
+        <f t="shared" ref="B300:B301" si="10">"(대화 주제) "&amp;E300&amp;" (남은 질문) "&amp;D300&amp;" (사용자 답변) "&amp;C300</f>
+        <v>(대화 주제) 마지막 할 말 (남은 질문) 마지막 할 말 (사용자 답변) 로라야 사랑해</v>
+      </c>
+      <c r="C300" t="s">
+        <v>589</v>
+      </c>
+      <c r="D300" t="s">
+        <v>482</v>
+      </c>
+      <c r="E300" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="301" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A301" t="s">
+        <v>539</v>
+      </c>
+      <c r="B301" t="str">
+        <f t="shared" si="10"/>
+        <v>(대화 주제) 마지막 할 말 (남은 질문) 마지막 할 말 (사용자 답변) 로라야 너의 예쁜 미모에 반했어</v>
+      </c>
+      <c r="C301" t="s">
+        <v>590</v>
+      </c>
+      <c r="D301" t="s">
+        <v>482</v>
+      </c>
+      <c r="E301" t="s">
+        <v>482</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FIX: ML interview question dataset
</commit_message>
<xml_diff>
--- a/2025_07_02_OhLoRA_ML_Tutor/ai_interview/dataset/all_train_and_test_data.xlsx
+++ b/2025_07_02_OhLoRA_ML_Tutor/ai_interview/dataset/all_train_and_test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AI_Projects\2025_07_02_OhLoRA_ML_Tutor\ai_interview\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{114AB604-8D21-45B7-9567-9C9265121FF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE5C1951-44E6-4D9D-8C48-8AC5CAEAFDEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18816" xr2:uid="{36F7775B-6BB8-4B8D-957C-E8DB745DD279}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1922" uniqueCount="591">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1929" uniqueCount="591">
   <si>
     <t>output_data</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -6523,9 +6523,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1D2CB62-8799-47EC-8115-E6B63AEE2C35}">
   <dimension ref="A1:I301"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A234" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B260" sqref="B260"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F110" sqref="F110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -6625,6 +6625,9 @@
       <c r="F5" t="s">
         <v>8</v>
       </c>
+      <c r="G5" t="s">
+        <v>6</v>
+      </c>
       <c r="H5" t="s">
         <v>6</v>
       </c>
@@ -6646,6 +6649,9 @@
       <c r="F6" t="s">
         <v>9</v>
       </c>
+      <c r="G6" t="s">
+        <v>6</v>
+      </c>
       <c r="H6" t="s">
         <v>6</v>
       </c>
@@ -6667,6 +6673,9 @@
       <c r="F7" t="s">
         <v>12</v>
       </c>
+      <c r="G7" t="s">
+        <v>6</v>
+      </c>
       <c r="H7" t="s">
         <v>6</v>
       </c>
@@ -6688,6 +6697,9 @@
       <c r="F8" t="s">
         <v>17</v>
       </c>
+      <c r="G8" t="s">
+        <v>6</v>
+      </c>
       <c r="H8" t="s">
         <v>18</v>
       </c>
@@ -6709,6 +6721,9 @@
       <c r="F9" t="s">
         <v>20</v>
       </c>
+      <c r="G9" t="s">
+        <v>6</v>
+      </c>
       <c r="H9" t="s">
         <v>18</v>
       </c>
@@ -6730,6 +6745,9 @@
       <c r="F10" t="s">
         <v>21</v>
       </c>
+      <c r="G10" t="s">
+        <v>6</v>
+      </c>
       <c r="H10" t="s">
         <v>18</v>
       </c>
@@ -6751,6 +6769,9 @@
       <c r="F11" t="s">
         <v>22</v>
       </c>
+      <c r="G11" t="s">
+        <v>6</v>
+      </c>
       <c r="H11" t="s">
         <v>18</v>
       </c>
@@ -9614,7 +9635,7 @@
         <v>329</v>
       </c>
       <c r="H117" t="s">
-        <v>240</v>
+        <v>257</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.4">
@@ -9641,7 +9662,7 @@
         <v>329</v>
       </c>
       <c r="H118" t="s">
-        <v>240</v>
+        <v>257</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.4">
@@ -9668,7 +9689,7 @@
         <v>329</v>
       </c>
       <c r="H119" t="s">
-        <v>240</v>
+        <v>257</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.4">
@@ -9695,7 +9716,7 @@
         <v>329</v>
       </c>
       <c r="H120" t="s">
-        <v>240</v>
+        <v>257</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.4">
@@ -9722,7 +9743,7 @@
         <v>329</v>
       </c>
       <c r="H121" t="s">
-        <v>240</v>
+        <v>257</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.4">
@@ -9749,7 +9770,7 @@
         <v>329</v>
       </c>
       <c r="H122" t="s">
-        <v>240</v>
+        <v>257</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.4">
@@ -9776,7 +9797,7 @@
         <v>258</v>
       </c>
       <c r="H123" t="s">
-        <v>240</v>
+        <v>257</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.4">
@@ -9803,7 +9824,7 @@
         <v>258</v>
       </c>
       <c r="H124" t="s">
-        <v>240</v>
+        <v>257</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.4">
@@ -9830,7 +9851,7 @@
         <v>258</v>
       </c>
       <c r="H125" t="s">
-        <v>240</v>
+        <v>257</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.4">
@@ -9938,7 +9959,7 @@
         <v>39</v>
       </c>
       <c r="H129" t="s">
-        <v>240</v>
+        <v>257</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.4">
@@ -9965,7 +9986,7 @@
         <v>39</v>
       </c>
       <c r="H130" t="s">
-        <v>240</v>
+        <v>257</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.4">
@@ -9992,7 +10013,7 @@
         <v>39</v>
       </c>
       <c r="H131" t="s">
-        <v>240</v>
+        <v>257</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.4">
@@ -10019,7 +10040,7 @@
         <v>39</v>
       </c>
       <c r="H132" t="s">
-        <v>240</v>
+        <v>257</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.4">
@@ -10046,7 +10067,7 @@
         <v>39</v>
       </c>
       <c r="H133" t="s">
-        <v>240</v>
+        <v>257</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.4">
@@ -10073,7 +10094,7 @@
         <v>39</v>
       </c>
       <c r="H134" t="s">
-        <v>240</v>
+        <v>257</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.4">
@@ -10100,7 +10121,7 @@
         <v>39</v>
       </c>
       <c r="H135" t="s">
-        <v>240</v>
+        <v>257</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.4">
@@ -10127,7 +10148,7 @@
         <v>39</v>
       </c>
       <c r="H136" t="s">
-        <v>240</v>
+        <v>257</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.4">
@@ -10154,7 +10175,7 @@
         <v>258</v>
       </c>
       <c r="H137" t="s">
-        <v>240</v>
+        <v>257</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.4">
@@ -10181,7 +10202,7 @@
         <v>258</v>
       </c>
       <c r="H138" t="s">
-        <v>240</v>
+        <v>257</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.4">
@@ -10208,7 +10229,7 @@
         <v>258</v>
       </c>
       <c r="H139" t="s">
-        <v>240</v>
+        <v>257</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
UPDATE: remaining answer value of interview start
</commit_message>
<xml_diff>
--- a/2025_07_02_OhLoRA_ML_Tutor/ai_interview/dataset/all_train_and_test_data.xlsx
+++ b/2025_07_02_OhLoRA_ML_Tutor/ai_interview/dataset/all_train_and_test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AI_Projects\2025_07_02_OhLoRA_ML_Tutor\ai_interview\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE5C1951-44E6-4D9D-8C48-8AC5CAEAFDEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F044FF7B-6DA0-4DBA-BEE9-8C85CE02041F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18816" xr2:uid="{36F7775B-6BB8-4B8D-957C-E8DB745DD279}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1929" uniqueCount="591">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1946" uniqueCount="591">
   <si>
     <t>output_data</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -6524,8 +6524,8 @@
   <dimension ref="A1:I301"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F110" sqref="F110"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -6619,6 +6619,9 @@
       <c r="C5" t="s">
         <v>7</v>
       </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
       <c r="E5" t="s">
         <v>6</v>
       </c>
@@ -6643,6 +6646,9 @@
       <c r="C6" t="s">
         <v>10</v>
       </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
       <c r="E6" t="s">
         <v>6</v>
       </c>
@@ -6667,6 +6673,9 @@
       <c r="C7" t="s">
         <v>11</v>
       </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
       <c r="E7" t="s">
         <v>6</v>
       </c>
@@ -6691,6 +6700,9 @@
       <c r="C8" t="s">
         <v>14</v>
       </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
       <c r="E8" t="s">
         <v>6</v>
       </c>
@@ -6715,6 +6727,9 @@
       <c r="C9" t="s">
         <v>13</v>
       </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
       <c r="E9" t="s">
         <v>6</v>
       </c>
@@ -6739,6 +6754,9 @@
       <c r="C10" t="s">
         <v>15</v>
       </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
       <c r="E10" t="s">
         <v>6</v>
       </c>
@@ -6763,6 +6781,9 @@
       <c r="C11" t="s">
         <v>16</v>
       </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
       <c r="E11" t="s">
         <v>6</v>
       </c>
@@ -13224,6 +13245,12 @@
       <c r="E251" t="s">
         <v>6</v>
       </c>
+      <c r="G251" t="s">
+        <v>6</v>
+      </c>
+      <c r="H251" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="252" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A252" t="s">
@@ -13239,6 +13266,12 @@
       <c r="E252" t="s">
         <v>6</v>
       </c>
+      <c r="G252" t="s">
+        <v>6</v>
+      </c>
+      <c r="H252" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="253" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A253" t="s">
@@ -13254,6 +13287,12 @@
       <c r="E253" t="s">
         <v>6</v>
       </c>
+      <c r="G253" t="s">
+        <v>6</v>
+      </c>
+      <c r="H253" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="254" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A254" t="s">
@@ -13269,6 +13308,12 @@
       <c r="E254" t="s">
         <v>6</v>
       </c>
+      <c r="G254" t="s">
+        <v>6</v>
+      </c>
+      <c r="H254" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="255" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A255" t="s">
@@ -13283,6 +13328,12 @@
       </c>
       <c r="E255" t="s">
         <v>6</v>
+      </c>
+      <c r="G255" t="s">
+        <v>6</v>
+      </c>
+      <c r="H255" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="256" spans="1:8" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
FIX: valid dataset (real experience part)
</commit_message>
<xml_diff>
--- a/2025_07_02_OhLoRA_ML_Tutor/ai_interview/dataset/all_train_and_test_data.xlsx
+++ b/2025_07_02_OhLoRA_ML_Tutor/ai_interview/dataset/all_train_and_test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AI_Projects\2025_07_02_OhLoRA_ML_Tutor\ai_interview\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A81D9A93-84D9-49AE-A428-3124859C871F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC05BC90-83E0-442A-866C-CA0D2B05EFA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18816" xr2:uid="{36F7775B-6BB8-4B8D-957C-E8DB745DD279}"/>
   </bookViews>
@@ -7155,9 +7155,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1D2CB62-8799-47EC-8115-E6B63AEE2C35}">
   <dimension ref="A1:I454"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A385" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B425" sqref="B425"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A230" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F264" sqref="F264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -18372,7 +18372,7 @@
         <v>39</v>
       </c>
       <c r="H438" t="s">
-        <v>345</v>
+        <v>390</v>
       </c>
     </row>
     <row r="439" spans="1:8" x14ac:dyDescent="0.4">
@@ -18420,7 +18420,7 @@
         <v>39</v>
       </c>
       <c r="H440" t="s">
-        <v>345</v>
+        <v>390</v>
       </c>
     </row>
     <row r="441" spans="1:8" x14ac:dyDescent="0.4">

</xml_diff>